<commit_message>
Creating the "good" template
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="236">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -110,6 +110,9 @@
     <t>Date Begin</t>
   </si>
   <si>
+    <t>Date end</t>
+  </si>
+  <si>
     <t>Dates Type</t>
   </si>
   <si>
@@ -326,9 +329,15 @@
     <t>The container indicator (e.g., number)</t>
   </si>
   <si>
+    <t>Top Container [indicator]</t>
+  </si>
+  <si>
     <t>Dates</t>
   </si>
   <si>
+    <t>Resource Identifier</t>
+  </si>
+  <si>
     <t>The Resource "Identifier", aka collection-level unit_id, OR, could be internal resource record number from URL.</t>
   </si>
   <si>
@@ -342,6 +351,9 @@
   </si>
   <si>
     <t>Unit_id</t>
+  </si>
+  <si>
+    <t>Component Unique Identifier</t>
   </si>
   <si>
     <t>unit_id</t>
@@ -647,6 +659,15 @@
     <t>Creator CorporateRelator</t>
   </si>
   <si>
+    <t>Family Agent header string</t>
+  </si>
+  <si>
+    <t>Family/Creator Relator</t>
+  </si>
+  <si>
+    <t>Corporate Agent header string</t>
+  </si>
+  <si>
     <t>Subject Source
 (If the subject term is created through this ingest, the source will  default to "Unspecified ingested source" unless the supplied Source value exactly matches an existing  controlled Source term.)</t>
   </si>
@@ -696,6 +717,12 @@
     <t>Corporate/Creator Relator(2)</t>
   </si>
   <si>
+    <t>Corporate Agent Record ID(2)</t>
+  </si>
+  <si>
+    <t>Corporate Agent header string(2)</t>
+  </si>
+  <si>
     <t>people_agent_record_id_1</t>
   </si>
   <si>
@@ -708,62 +735,14 @@
     <t>families_agent_relator_1</t>
   </si>
   <si>
-    <t>Resource Identifier (not used)</t>
-  </si>
-  <si>
-    <t>Barcode</t>
-  </si>
-  <si>
-    <t>Top Container indicator</t>
-  </si>
-  <si>
-    <t>Family Agent/Creator Record ID</t>
-  </si>
-  <si>
-    <t>Family Agent/Creator header string</t>
-  </si>
-  <si>
-    <t>Corporate Agent/Creator Record ID</t>
-  </si>
-  <si>
-    <t>Corporate Agent/Creator header string</t>
-  </si>
-  <si>
-    <t>Corporate Agent/Creator Record ID(2)</t>
-  </si>
-  <si>
-    <t>Corporate Agent/Creator header string(2)</t>
-  </si>
-  <si>
-    <t>Corporate Agent/Creator Relator(2)</t>
-  </si>
-  <si>
-    <t>Family Agent/Creator Relator</t>
-  </si>
-  <si>
-    <t>Component Unit Identifier</t>
-  </si>
-  <si>
-    <t>Date End</t>
-  </si>
-  <si>
-    <t>Date Expression</t>
-  </si>
-  <si>
-    <t>instance type: Accession, Audio, Books, etc.</t>
-  </si>
-  <si>
-    <t>Container Instance Type</t>
-  </si>
-  <si>
-    <t>cont_instance_type</t>
+    <t>This is the template for importing using aspace-import-excel.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -863,20 +842,6 @@
     <font>
       <i/>
       <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1043,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1102,6 +1067,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1212,12 +1180,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1595,19 +1557,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ANZ6"/>
+  <dimension ref="A1:ANY7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X3" sqref="X3"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="36" customWidth="1"/>
-    <col min="2" max="2" width="0" style="20" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" style="37" customWidth="1"/>
+    <col min="2" max="2" width="16" style="21"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
@@ -1615,7 +1577,7 @@
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="1"/>
     <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="53" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="54" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
@@ -1623,1016 +1585,1007 @@
     <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="23" width="26.85546875" style="1" customWidth="1"/>
-    <col min="24" max="24" width="23" style="1"/>
-    <col min="25" max="25" width="16.5703125" style="1" customWidth="1"/>
-    <col min="26" max="26" width="23" style="1"/>
-    <col min="27" max="27" width="10.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" style="1" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" style="1" customWidth="1"/>
-    <col min="33" max="34" width="9.140625" style="1"/>
-    <col min="35" max="35" width="15.28515625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="22.7109375" style="1"/>
-    <col min="37" max="37" width="13" style="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.7109375" style="1"/>
-    <col min="40" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="15.140625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="20.140625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="12.85546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" style="1"/>
-    <col min="45" max="45" width="11.42578125" style="1" customWidth="1"/>
-    <col min="46" max="47" width="9.140625" style="1"/>
-    <col min="48" max="48" width="22.7109375" style="1"/>
-    <col min="49" max="52" width="9.140625" style="1"/>
-    <col min="53" max="53" width="11.5703125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="12.28515625" style="1" customWidth="1"/>
-    <col min="55" max="57" width="13.5703125" style="1" customWidth="1"/>
-    <col min="58" max="59" width="10.85546875" style="1" customWidth="1"/>
-    <col min="60" max="60" width="15.42578125" style="1" customWidth="1"/>
-    <col min="61" max="61" width="9.28515625" style="1"/>
-    <col min="62" max="62" width="17" style="1" customWidth="1"/>
-    <col min="63" max="63" width="12.28515625" style="1" customWidth="1"/>
-    <col min="64" max="64" width="11.7109375" style="1" customWidth="1"/>
-    <col min="65" max="65" width="16" style="1" customWidth="1"/>
-    <col min="66" max="66" width="9.140625" style="1"/>
-    <col min="67" max="67" width="12" customWidth="1"/>
-    <col min="68" max="72" width="11.85546875" style="1" customWidth="1"/>
-    <col min="73" max="73" width="14.85546875" style="1" customWidth="1"/>
-    <col min="74" max="74" width="12.28515625" style="1" customWidth="1"/>
-    <col min="75" max="76" width="9.140625" style="1"/>
-    <col min="77" max="77" width="18.42578125" style="1" customWidth="1"/>
-    <col min="78" max="78" width="10.140625" style="1" customWidth="1"/>
-    <col min="79" max="1066" width="9.28515625" style="1"/>
+    <col min="24" max="25" width="23" style="1"/>
+    <col min="26" max="26" width="10.42578125" style="1" customWidth="1"/>
+    <col min="27" max="27" width="19" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19.140625" style="1" customWidth="1"/>
+    <col min="29" max="29" width="10.42578125" style="1" customWidth="1"/>
+    <col min="30" max="30" width="11.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" style="1" customWidth="1"/>
+    <col min="32" max="33" width="9.140625" style="1"/>
+    <col min="34" max="34" width="15.28515625" style="1" customWidth="1"/>
+    <col min="35" max="35" width="22.7109375" style="1"/>
+    <col min="36" max="36" width="13" style="1" customWidth="1"/>
+    <col min="37" max="37" width="15.42578125" style="1" customWidth="1"/>
+    <col min="38" max="38" width="22.7109375" style="1"/>
+    <col min="39" max="39" width="9.140625" style="1"/>
+    <col min="40" max="40" width="15.140625" style="1" customWidth="1"/>
+    <col min="41" max="41" width="20.140625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="12.85546875" style="1" customWidth="1"/>
+    <col min="43" max="43" width="9.140625" style="1"/>
+    <col min="44" max="44" width="11.42578125" style="1" customWidth="1"/>
+    <col min="45" max="46" width="9.140625" style="1"/>
+    <col min="47" max="47" width="22.7109375" style="1"/>
+    <col min="48" max="51" width="9.140625" style="1"/>
+    <col min="52" max="52" width="11.5703125" style="1" customWidth="1"/>
+    <col min="53" max="53" width="12.28515625" style="1" customWidth="1"/>
+    <col min="54" max="56" width="13.5703125" style="1" customWidth="1"/>
+    <col min="57" max="58" width="10.85546875" style="1" customWidth="1"/>
+    <col min="59" max="59" width="15.42578125" style="1" customWidth="1"/>
+    <col min="60" max="60" width="9.28515625" style="1"/>
+    <col min="61" max="61" width="17" style="1" customWidth="1"/>
+    <col min="62" max="62" width="12.28515625" style="1" customWidth="1"/>
+    <col min="63" max="63" width="11.7109375" style="1" customWidth="1"/>
+    <col min="64" max="64" width="16" style="1" customWidth="1"/>
+    <col min="65" max="65" width="9.140625" style="1"/>
+    <col min="66" max="66" width="12" customWidth="1"/>
+    <col min="67" max="71" width="11.85546875" style="1" customWidth="1"/>
+    <col min="72" max="72" width="14.85546875" style="1" customWidth="1"/>
+    <col min="73" max="73" width="12.28515625" style="1" customWidth="1"/>
+    <col min="74" max="75" width="9.140625" style="1"/>
+    <col min="76" max="76" width="18.42578125" style="1" customWidth="1"/>
+    <col min="77" max="77" width="10.140625" style="1" customWidth="1"/>
+    <col min="78" max="1065" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+    <row r="1" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:77" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="M2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="N2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="O2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="P2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q2" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="T2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="U2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="V2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="W2" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AB2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AD2" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="AF2" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH2" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="AI2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AJ2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AK2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AL2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AN2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AO2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AP2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AR2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AV2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AY2" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BA2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BB2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BE2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BF2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BG2" s="25" t="s">
+        <v>135</v>
+      </c>
+      <c r="BH2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BI2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BJ2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BK2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BL2" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="BM2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BN2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BO2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BP2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BQ2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BR2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BS2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BT2" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BV2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BW2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX2" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="BY2" s="35" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:77" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="40" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>181</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="J3" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="N3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="W3" s="43" t="s">
+        <v>40</v>
+      </c>
+      <c r="X3" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="Y3" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="AE3" s="30" t="s">
+        <v>83</v>
+      </c>
+      <c r="AF3" s="31" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG3" s="30" t="s">
+        <v>85</v>
+      </c>
+      <c r="AH3" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="AI3" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="AJ3" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="AK3" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="AL3" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="AM3" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="AN3" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="AO3" s="33" t="s">
+        <v>204</v>
+      </c>
+      <c r="AP3" s="33" t="s">
+        <v>201</v>
+      </c>
+      <c r="AQ3" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="AR3" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="AS3" s="33" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT3" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU3" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="AV3" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="AW3" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX3" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="AY3" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="AZ3" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="BA3" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="BB3" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC3" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="BD3" s="33" t="s">
+        <v>183</v>
+      </c>
+      <c r="BE3" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="BF3" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="BG3" s="33" t="s">
+        <v>213</v>
+      </c>
+      <c r="BH3" s="32" t="s">
+        <v>154</v>
+      </c>
+      <c r="BI3" s="32" t="s">
+        <v>155</v>
+      </c>
+      <c r="BJ3" s="32" t="s">
+        <v>156</v>
+      </c>
+      <c r="BK3" s="32" t="s">
+        <v>157</v>
+      </c>
+      <c r="BL3" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="BM3" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="BN3" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="BO3" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="BP3" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="BQ3" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="BR3" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="BS3" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="BT3" s="32" t="s">
+        <v>168</v>
+      </c>
+      <c r="BU3" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="BV3" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="BW3" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="BX3" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="BY3" s="32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77" s="50" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>79</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="46" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="46" t="s">
+        <v>81</v>
+      </c>
+      <c r="R4" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="S4" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="46" t="s">
+        <v>148</v>
+      </c>
+      <c r="V4" s="46" t="s">
+        <v>42</v>
+      </c>
+      <c r="W4" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="X4" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y4" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z4" s="46" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA4" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="AB4" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="AC4" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="AD4" s="46" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE4" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="AF4" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH4" s="46" t="s">
+        <v>231</v>
+      </c>
+      <c r="AI4" s="46" t="s">
+        <v>214</v>
+      </c>
+      <c r="AJ4" s="46" t="s">
+        <v>215</v>
+      </c>
+      <c r="AK4" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="AL4" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="AM4" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN4" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="AO4" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="AP4" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="AQ4" s="46" t="s">
+        <v>232</v>
+      </c>
+      <c r="AR4" s="46" t="s">
+        <v>233</v>
+      </c>
+      <c r="AS4" s="46" t="s">
+        <v>234</v>
+      </c>
+      <c r="AT4" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU4" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="AV4" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="AW4" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="AX4" s="46" t="s">
+        <v>227</v>
+      </c>
+      <c r="AY4" s="46" t="s">
+        <v>226</v>
+      </c>
+      <c r="AZ4" s="46" t="s">
+        <v>184</v>
+      </c>
+      <c r="BA4" s="46" t="s">
+        <v>138</v>
+      </c>
+      <c r="BB4" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="BC4" s="46" t="s">
+        <v>186</v>
+      </c>
+      <c r="BD4" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="BE4" s="46" t="s">
+        <v>140</v>
+      </c>
+      <c r="BF4" s="46" t="s">
+        <v>141</v>
+      </c>
+      <c r="BG4" s="46" t="s">
+        <v>187</v>
+      </c>
+      <c r="BH4" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="BI4" s="46" t="s">
+        <v>61</v>
+      </c>
+      <c r="BJ4" s="49" t="s">
+        <v>64</v>
+      </c>
+      <c r="BK4" s="46" t="s">
+        <v>59</v>
+      </c>
+      <c r="BL4" s="46" t="s">
+        <v>60</v>
+      </c>
+      <c r="BM4" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN4" s="49" t="s">
+        <v>129</v>
+      </c>
+      <c r="BO4" s="49" t="s">
+        <v>67</v>
+      </c>
+      <c r="BP4" s="49" t="s">
+        <v>65</v>
+      </c>
+      <c r="BQ4" s="46" t="s">
+        <v>62</v>
+      </c>
+      <c r="BR4" s="46" t="s">
+        <v>130</v>
+      </c>
+      <c r="BS4" s="46" t="s">
+        <v>131</v>
+      </c>
+      <c r="BT4" s="49" t="s">
+        <v>95</v>
+      </c>
+      <c r="BU4" s="46" t="s">
+        <v>58</v>
+      </c>
+      <c r="BV4" s="49" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW4" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX4" s="49" t="s">
+        <v>68</v>
+      </c>
+      <c r="BY4" s="49" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:77" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="50" t="s">
-        <v>103</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="M1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="N1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="O1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="P1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q1" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="W1" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="X1" s="25" t="s">
+      <c r="C5" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="J5" s="55" t="s">
+        <v>179</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="R5" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="U5" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="V5" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="W5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="X5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Y1" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="Z1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AG1" s="27" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH1" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI1" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AK1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AL1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AM1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AN1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AO1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AP1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AQ1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AR1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AS1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AT1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AU1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AV1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AX1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AY1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AZ1" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="BA1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BB1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BC1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BD1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BE1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BF1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BG1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="BI1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BJ1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BK1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BL1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BM1" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="BN1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BO1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BP1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BQ1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BR1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BS1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BT1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BU1" s="35" t="s">
-        <v>69</v>
-      </c>
-      <c r="BV1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BW1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BY1" s="34" t="s">
-        <v>69</v>
-      </c>
-      <c r="BZ1" s="34" t="s">
-        <v>69</v>
+      <c r="Y5" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="Z5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="AA5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB5" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC5" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE5" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="AF5" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG5" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AI5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="BF5" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BG5" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="BJ5" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="BK5" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="BL5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="BM5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BN5" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="BO5" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="BP5" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="BQ5" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="BR5" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="BS5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BT5" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="BU5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="BV5" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="BW5" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="BX5" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="BY5" s="7" t="s">
+        <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:78" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>109</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="G2" s="19" t="s">
-        <v>177</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>178</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>116</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="S2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="T2" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="W2" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="X2" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="Y2" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="15" t="s">
-        <v>100</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD2" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE2" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF2" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG2" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH2" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI2" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="AJ2" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="AK2" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="AL2" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="AM2" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="AN2" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO2" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP2" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="AQ2" s="32" t="s">
-        <v>197</v>
-      </c>
-      <c r="AR2" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="AS2" s="32" t="s">
-        <v>201</v>
-      </c>
-      <c r="AT2" s="32" t="s">
-        <v>203</v>
-      </c>
-      <c r="AU2" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="AV2" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="AW2" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="AX2" s="32" t="s">
-        <v>204</v>
-      </c>
-      <c r="AY2" s="32" t="s">
-        <v>202</v>
-      </c>
-      <c r="AZ2" s="32" t="s">
-        <v>205</v>
-      </c>
-      <c r="BA2" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="BB2" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="BC2" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="BD2" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="BE2" s="32" t="s">
-        <v>179</v>
-      </c>
-      <c r="BF2" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="BG2" s="32" t="s">
-        <v>133</v>
-      </c>
-      <c r="BH2" s="32" t="s">
-        <v>206</v>
-      </c>
-      <c r="BI2" s="31" t="s">
-        <v>150</v>
-      </c>
-      <c r="BJ2" s="31" t="s">
-        <v>151</v>
-      </c>
-      <c r="BK2" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="BL2" s="31" t="s">
-        <v>153</v>
-      </c>
-      <c r="BM2" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="BN2" s="31" t="s">
-        <v>155</v>
-      </c>
-      <c r="BO2" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="BP2" s="31" t="s">
-        <v>157</v>
-      </c>
-      <c r="BQ2" s="31" t="s">
-        <v>159</v>
-      </c>
-      <c r="BR2" s="31" t="s">
-        <v>160</v>
-      </c>
-      <c r="BS2" s="31" t="s">
-        <v>162</v>
-      </c>
-      <c r="BT2" s="31" t="s">
-        <v>163</v>
-      </c>
-      <c r="BU2" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="BV2" s="31" t="s">
-        <v>165</v>
-      </c>
-      <c r="BW2" s="31" t="s">
-        <v>166</v>
-      </c>
-      <c r="BX2" s="31" t="s">
-        <v>168</v>
-      </c>
-      <c r="BY2" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="BZ2" s="31" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="3" spans="1:78" s="49" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="46" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="47" t="s">
-        <v>75</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="48" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="H3" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="45" t="s">
-        <v>130</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="K3" s="45" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="M3" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="N3" s="45" t="s">
-        <v>27</v>
-      </c>
-      <c r="O3" s="45" t="s">
-        <v>21</v>
-      </c>
-      <c r="P3" s="45" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" s="45" t="s">
-        <v>80</v>
-      </c>
-      <c r="R3" s="45" t="s">
-        <v>89</v>
-      </c>
-      <c r="S3" s="45" t="s">
-        <v>23</v>
-      </c>
-      <c r="T3" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="U3" s="45" t="s">
-        <v>144</v>
-      </c>
-      <c r="V3" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="W3" s="48" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" s="45" t="s">
-        <v>242</v>
-      </c>
-      <c r="Y3" s="45" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z3" s="45" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA3" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB3" s="45" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC3" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD3" s="45" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE3" s="45" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF3" s="45" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG3" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH3" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI3" s="45" t="s">
-        <v>222</v>
-      </c>
-      <c r="AJ3" s="45" t="s">
-        <v>207</v>
-      </c>
-      <c r="AK3" s="45" t="s">
-        <v>208</v>
-      </c>
-      <c r="AL3" s="45" t="s">
-        <v>209</v>
-      </c>
-      <c r="AM3" s="45" t="s">
-        <v>210</v>
-      </c>
-      <c r="AN3" s="45" t="s">
-        <v>211</v>
-      </c>
-      <c r="AO3" s="45" t="s">
-        <v>212</v>
-      </c>
-      <c r="AP3" s="45" t="s">
-        <v>213</v>
-      </c>
-      <c r="AQ3" s="45" t="s">
-        <v>214</v>
-      </c>
-      <c r="AR3" s="45" t="s">
-        <v>223</v>
-      </c>
-      <c r="AS3" s="45" t="s">
-        <v>224</v>
-      </c>
-      <c r="AT3" s="45" t="s">
-        <v>225</v>
-      </c>
-      <c r="AU3" s="45" t="s">
-        <v>215</v>
-      </c>
-      <c r="AV3" s="45" t="s">
-        <v>216</v>
-      </c>
-      <c r="AW3" s="45" t="s">
-        <v>217</v>
-      </c>
-      <c r="AX3" s="45" t="s">
-        <v>218</v>
-      </c>
-      <c r="AY3" s="45" t="s">
-        <v>220</v>
-      </c>
-      <c r="AZ3" s="45" t="s">
-        <v>219</v>
-      </c>
-      <c r="BA3" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="BB3" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="BC3" s="45" t="s">
-        <v>135</v>
-      </c>
-      <c r="BD3" s="45" t="s">
-        <v>182</v>
-      </c>
-      <c r="BE3" s="45" t="s">
-        <v>181</v>
-      </c>
-      <c r="BF3" s="45" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG3" s="45" t="s">
-        <v>137</v>
-      </c>
-      <c r="BH3" s="45" t="s">
-        <v>183</v>
-      </c>
-      <c r="BI3" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ3" s="45" t="s">
-        <v>60</v>
-      </c>
-      <c r="BK3" s="48" t="s">
-        <v>63</v>
-      </c>
-      <c r="BL3" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="BM3" s="45" t="s">
-        <v>59</v>
-      </c>
-      <c r="BN3" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="BO3" s="48" t="s">
-        <v>125</v>
-      </c>
-      <c r="BP3" s="48" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ3" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR3" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="BS3" s="45" t="s">
-        <v>126</v>
-      </c>
-      <c r="BT3" s="45" t="s">
-        <v>127</v>
-      </c>
-      <c r="BU3" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="BV3" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="BW3" s="48" t="s">
-        <v>68</v>
-      </c>
-      <c r="BX3" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY3" s="48" t="s">
-        <v>67</v>
-      </c>
-      <c r="BZ3" s="48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:78" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
-        <v>72</v>
-      </c>
-      <c r="B4" s="57" t="s">
-        <v>226</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="58" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="J4" s="54" t="s">
-        <v>175</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="R4" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="U4" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="V4" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="W4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="X4" s="4" t="s">
-        <v>241</v>
-      </c>
-      <c r="Y4" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z4" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="AA4" s="4" t="s">
-        <v>227</v>
-      </c>
-      <c r="AB4" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC4" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AD4" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="AE4" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AF4" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AG4" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH4" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI4" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="AJ4" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="AK4" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="AL4" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="AM4" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="AN4" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="AO4" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="AP4" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="AQ4" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AR4" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AS4" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AT4" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="AU4" s="4" t="s">
-        <v>231</v>
-      </c>
-      <c r="AV4" s="4" t="s">
-        <v>232</v>
-      </c>
-      <c r="AW4" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="AX4" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="AY4" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="AZ4" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="BA4" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="BB4" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="BC4" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="BE4" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="BF4" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="BG4" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="BH4" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="BI4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="BJ4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="BK4" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="BL4" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="BM4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="BN4" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="BO4" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="BP4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="BQ4" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="BR4" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="BS4" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="BT4" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="BU4" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="BV4" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW4" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="BX4" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="BY4" s="7" t="s">
-        <v>171</v>
-      </c>
-      <c r="BZ4" s="7" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="5" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="G6" s="37"/>
+    <row r="6" spans="1:77" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+      <c r="G7" s="38"/>
     </row>
   </sheetData>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H5:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576">
       <formula1>"Class,Collection,File,Fonds,Item,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J1048576">
-      <formula1>"false,true"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576">
+      <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O5:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O1048576">
       <formula1>"bulk,single,inclusive"</formula1>
     </dataValidation>
-    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G5:G1048576">
+    <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G6:G1048576">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I5:I1048576">
-      <formula1>"false,true"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I6:I1048576">
+      <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2655,43 +2608,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>111</v>
+      <c r="A1" s="23" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
-        <v>148</v>
+      <c r="A7" s="56" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -2708,43 +2661,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142" style="43" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="142" style="44" bestFit="1" customWidth="1"/>
     <col min="2" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="43" t="s">
-        <v>122</v>
+      <c r="A1" s="44" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="43" t="s">
-        <v>121</v>
+      <c r="A3" s="44" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
-        <v>110</v>
+      <c r="A4" s="44" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43" t="s">
-        <v>118</v>
+      <c r="A5" s="44" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43" t="s">
-        <v>117</v>
+      <c r="A6" s="44" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43" t="s">
-        <v>119</v>
+      <c r="A7" s="44" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43" t="s">
-        <v>120</v>
+      <c r="A8" s="44" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Container instance type back in
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="239">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -736,6 +736,15 @@
   </si>
   <si>
     <t>This is the template for importing using aspace-import-excel.  You may replace this line with something of your choosing after you've copied the file for your use.</t>
+  </si>
+  <si>
+    <t>instance type: Accession, Audio, Books, etc.</t>
+  </si>
+  <si>
+    <t>cont_instance_type</t>
+  </si>
+  <si>
+    <t>Container Instance Type</t>
   </si>
 </sst>
 </file>
@@ -1557,13 +1566,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ANY7"/>
+  <dimension ref="A1:ANZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="Z3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="X2" sqref="X2:X5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1584,56 +1593,56 @@
     <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
     <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
-    <col min="17" max="23" width="26.85546875" style="1" customWidth="1"/>
-    <col min="24" max="25" width="23" style="1"/>
-    <col min="26" max="26" width="10.42578125" style="1" customWidth="1"/>
-    <col min="27" max="27" width="19" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19.140625" style="1" customWidth="1"/>
-    <col min="29" max="29" width="10.42578125" style="1" customWidth="1"/>
-    <col min="30" max="30" width="11.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="10.42578125" style="1" customWidth="1"/>
-    <col min="32" max="33" width="9.140625" style="1"/>
-    <col min="34" max="34" width="15.28515625" style="1" customWidth="1"/>
-    <col min="35" max="35" width="22.7109375" style="1"/>
-    <col min="36" max="36" width="13" style="1" customWidth="1"/>
-    <col min="37" max="37" width="15.42578125" style="1" customWidth="1"/>
-    <col min="38" max="38" width="22.7109375" style="1"/>
-    <col min="39" max="39" width="9.140625" style="1"/>
-    <col min="40" max="40" width="15.140625" style="1" customWidth="1"/>
-    <col min="41" max="41" width="20.140625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="12.85546875" style="1" customWidth="1"/>
-    <col min="43" max="43" width="9.140625" style="1"/>
-    <col min="44" max="44" width="11.42578125" style="1" customWidth="1"/>
-    <col min="45" max="46" width="9.140625" style="1"/>
-    <col min="47" max="47" width="22.7109375" style="1"/>
-    <col min="48" max="51" width="9.140625" style="1"/>
-    <col min="52" max="52" width="11.5703125" style="1" customWidth="1"/>
-    <col min="53" max="53" width="12.28515625" style="1" customWidth="1"/>
-    <col min="54" max="56" width="13.5703125" style="1" customWidth="1"/>
-    <col min="57" max="58" width="10.85546875" style="1" customWidth="1"/>
-    <col min="59" max="59" width="15.42578125" style="1" customWidth="1"/>
-    <col min="60" max="60" width="9.28515625" style="1"/>
-    <col min="61" max="61" width="17" style="1" customWidth="1"/>
-    <col min="62" max="62" width="12.28515625" style="1" customWidth="1"/>
-    <col min="63" max="63" width="11.7109375" style="1" customWidth="1"/>
-    <col min="64" max="64" width="16" style="1" customWidth="1"/>
-    <col min="65" max="65" width="9.140625" style="1"/>
-    <col min="66" max="66" width="12" customWidth="1"/>
-    <col min="67" max="71" width="11.85546875" style="1" customWidth="1"/>
-    <col min="72" max="72" width="14.85546875" style="1" customWidth="1"/>
-    <col min="73" max="73" width="12.28515625" style="1" customWidth="1"/>
-    <col min="74" max="75" width="9.140625" style="1"/>
-    <col min="76" max="76" width="18.42578125" style="1" customWidth="1"/>
-    <col min="77" max="77" width="10.140625" style="1" customWidth="1"/>
-    <col min="78" max="1065" width="9.28515625" style="1"/>
+    <col min="17" max="24" width="26.85546875" style="1" customWidth="1"/>
+    <col min="25" max="26" width="23" style="1"/>
+    <col min="27" max="27" width="10.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" style="1" customWidth="1"/>
+    <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="10.42578125" style="1" customWidth="1"/>
+    <col min="33" max="34" width="9.140625" style="1"/>
+    <col min="35" max="35" width="15.28515625" style="1" customWidth="1"/>
+    <col min="36" max="36" width="22.7109375" style="1"/>
+    <col min="37" max="37" width="13" style="1" customWidth="1"/>
+    <col min="38" max="38" width="15.42578125" style="1" customWidth="1"/>
+    <col min="39" max="39" width="22.7109375" style="1"/>
+    <col min="40" max="40" width="9.140625" style="1"/>
+    <col min="41" max="41" width="15.140625" style="1" customWidth="1"/>
+    <col min="42" max="42" width="20.140625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="12.85546875" style="1" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="1"/>
+    <col min="45" max="45" width="11.42578125" style="1" customWidth="1"/>
+    <col min="46" max="47" width="9.140625" style="1"/>
+    <col min="48" max="48" width="22.7109375" style="1"/>
+    <col min="49" max="52" width="9.140625" style="1"/>
+    <col min="53" max="53" width="11.5703125" style="1" customWidth="1"/>
+    <col min="54" max="54" width="12.28515625" style="1" customWidth="1"/>
+    <col min="55" max="57" width="13.5703125" style="1" customWidth="1"/>
+    <col min="58" max="59" width="10.85546875" style="1" customWidth="1"/>
+    <col min="60" max="60" width="15.42578125" style="1" customWidth="1"/>
+    <col min="61" max="61" width="9.28515625" style="1"/>
+    <col min="62" max="62" width="17" style="1" customWidth="1"/>
+    <col min="63" max="63" width="12.28515625" style="1" customWidth="1"/>
+    <col min="64" max="64" width="11.7109375" style="1" customWidth="1"/>
+    <col min="65" max="65" width="16" style="1" customWidth="1"/>
+    <col min="66" max="66" width="9.140625" style="1"/>
+    <col min="67" max="67" width="12" customWidth="1"/>
+    <col min="68" max="72" width="11.85546875" style="1" customWidth="1"/>
+    <col min="73" max="73" width="14.85546875" style="1" customWidth="1"/>
+    <col min="74" max="74" width="12.28515625" style="1" customWidth="1"/>
+    <col min="75" max="76" width="9.140625" style="1"/>
+    <col min="77" max="77" width="18.42578125" style="1" customWidth="1"/>
+    <col min="78" max="78" width="10.140625" style="1" customWidth="1"/>
+    <col min="79" max="1066" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="37" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="2" spans="1:77" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:78" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="39" t="s">
         <v>0</v>
       </c>
@@ -1706,7 +1715,7 @@
       <c r="X2" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="27" t="s">
+      <c r="Y2" s="26" t="s">
         <v>33</v>
       </c>
       <c r="Z2" s="27" t="s">
@@ -1724,20 +1733,20 @@
       <c r="AD2" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="28" t="s">
-        <v>45</v>
+      <c r="AE2" s="27" t="s">
+        <v>33</v>
       </c>
       <c r="AF2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AG2" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="AH2" s="57" t="s">
+      <c r="AH2" s="29" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI2" s="57" t="s">
         <v>93</v>
-      </c>
-      <c r="AI2" s="25" t="s">
-        <v>1</v>
       </c>
       <c r="AJ2" s="25" t="s">
         <v>1</v>
@@ -1788,7 +1797,7 @@
         <v>1</v>
       </c>
       <c r="AZ2" s="25" t="s">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="BA2" s="25" t="s">
         <v>135</v>
@@ -1811,8 +1820,8 @@
       <c r="BG2" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="BH2" s="35" t="s">
-        <v>70</v>
+      <c r="BH2" s="25" t="s">
+        <v>135</v>
       </c>
       <c r="BI2" s="35" t="s">
         <v>70</v>
@@ -1823,10 +1832,10 @@
       <c r="BK2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="BL2" s="34" t="s">
+      <c r="BL2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="BM2" s="35" t="s">
+      <c r="BM2" s="34" t="s">
         <v>70</v>
       </c>
       <c r="BN2" s="35" t="s">
@@ -1847,10 +1856,10 @@
       <c r="BS2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="BT2" s="36" t="s">
+      <c r="BT2" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="BU2" s="35" t="s">
+      <c r="BU2" s="36" t="s">
         <v>70</v>
       </c>
       <c r="BV2" s="35" t="s">
@@ -1865,8 +1874,11 @@
       <c r="BY2" s="35" t="s">
         <v>70</v>
       </c>
+      <c r="BZ2" s="35" t="s">
+        <v>70</v>
+      </c>
     </row>
-    <row r="3" spans="1:77" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:78" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="40" t="s">
         <v>74</v>
       </c>
@@ -1937,169 +1949,172 @@
         <v>40</v>
       </c>
       <c r="X3" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="Y3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="Y3" s="15" t="s">
+      <c r="Z3" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AA3" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="AA3" s="13" t="s">
+      <c r="AB3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AC3" s="13" t="s">
         <v>99</v>
       </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AD3" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="AD3" s="13" t="s">
+      <c r="AE3" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="AE3" s="30" t="s">
+      <c r="AF3" s="30" t="s">
         <v>83</v>
       </c>
-      <c r="AF3" s="31" t="s">
+      <c r="AG3" s="31" t="s">
         <v>82</v>
       </c>
-      <c r="AG3" s="30" t="s">
+      <c r="AH3" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="AH3" s="33" t="s">
+      <c r="AI3" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="AI3" s="33" t="s">
+      <c r="AJ3" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="AJ3" s="33" t="s">
+      <c r="AK3" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="AK3" s="33" t="s">
+      <c r="AL3" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="AL3" s="33" t="s">
+      <c r="AM3" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="AM3" s="33" t="s">
+      <c r="AN3" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="AN3" s="33" t="s">
+      <c r="AO3" s="33" t="s">
         <v>202</v>
       </c>
-      <c r="AO3" s="33" t="s">
+      <c r="AP3" s="33" t="s">
         <v>204</v>
       </c>
-      <c r="AP3" s="33" t="s">
+      <c r="AQ3" s="33" t="s">
         <v>201</v>
       </c>
-      <c r="AQ3" s="33" t="s">
+      <c r="AR3" s="33" t="s">
         <v>203</v>
       </c>
-      <c r="AR3" s="33" t="s">
+      <c r="AS3" s="33" t="s">
         <v>205</v>
       </c>
-      <c r="AS3" s="33" t="s">
+      <c r="AT3" s="33" t="s">
         <v>207</v>
       </c>
-      <c r="AT3" s="33" t="s">
+      <c r="AU3" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="AU3" s="33" t="s">
+      <c r="AV3" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="AV3" s="33" t="s">
+      <c r="AW3" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="AW3" s="33" t="s">
+      <c r="AX3" s="33" t="s">
         <v>208</v>
       </c>
-      <c r="AX3" s="33" t="s">
+      <c r="AY3" s="33" t="s">
         <v>206</v>
       </c>
-      <c r="AY3" s="33" t="s">
+      <c r="AZ3" s="33" t="s">
         <v>209</v>
       </c>
-      <c r="AZ3" s="33" t="s">
+      <c r="BA3" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="BA3" s="33" t="s">
+      <c r="BB3" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="BB3" s="33" t="s">
+      <c r="BC3" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="BC3" s="33" t="s">
+      <c r="BD3" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="BD3" s="33" t="s">
+      <c r="BE3" s="33" t="s">
         <v>183</v>
       </c>
-      <c r="BE3" s="33" t="s">
+      <c r="BF3" s="33" t="s">
         <v>136</v>
       </c>
-      <c r="BF3" s="33" t="s">
+      <c r="BG3" s="33" t="s">
         <v>137</v>
       </c>
-      <c r="BG3" s="33" t="s">
+      <c r="BH3" s="33" t="s">
         <v>213</v>
       </c>
-      <c r="BH3" s="32" t="s">
+      <c r="BI3" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="BI3" s="32" t="s">
+      <c r="BJ3" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="BJ3" s="32" t="s">
+      <c r="BK3" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="BK3" s="32" t="s">
+      <c r="BL3" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="BL3" s="32" t="s">
+      <c r="BM3" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="BM3" s="32" t="s">
+      <c r="BN3" s="32" t="s">
         <v>159</v>
       </c>
-      <c r="BN3" s="32" t="s">
+      <c r="BO3" s="32" t="s">
         <v>160</v>
       </c>
-      <c r="BO3" s="32" t="s">
+      <c r="BP3" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="BP3" s="32" t="s">
+      <c r="BQ3" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="BQ3" s="32" t="s">
+      <c r="BR3" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="BR3" s="32" t="s">
+      <c r="BS3" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="BS3" s="32" t="s">
+      <c r="BT3" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="BT3" s="32" t="s">
+      <c r="BU3" s="32" t="s">
         <v>168</v>
       </c>
-      <c r="BU3" s="32" t="s">
+      <c r="BV3" s="32" t="s">
         <v>169</v>
       </c>
-      <c r="BV3" s="32" t="s">
+      <c r="BW3" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="BW3" s="32" t="s">
+      <c r="BX3" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="BX3" s="32" t="s">
+      <c r="BY3" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="BY3" s="32" t="s">
+      <c r="BZ3" s="32" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="4" spans="1:77" s="50" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:78" s="50" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>5</v>
       </c>
@@ -2170,169 +2185,172 @@
         <v>41</v>
       </c>
       <c r="X4" s="46" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y4" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="Y4" s="46" t="s">
+      <c r="Z4" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="46" t="s">
+      <c r="AA4" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="AA4" s="46" t="s">
+      <c r="AB4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AB4" s="46" t="s">
+      <c r="AC4" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="AC4" s="46" t="s">
+      <c r="AD4" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="AD4" s="46" t="s">
+      <c r="AE4" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="AE4" s="46" t="s">
+      <c r="AF4" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="AF4" s="46" t="s">
+      <c r="AG4" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="AG4" s="46" t="s">
+      <c r="AH4" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="AH4" s="46" t="s">
+      <c r="AI4" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="AI4" s="46" t="s">
+      <c r="AJ4" s="46" t="s">
         <v>214</v>
       </c>
-      <c r="AJ4" s="46" t="s">
+      <c r="AK4" s="46" t="s">
         <v>215</v>
       </c>
-      <c r="AK4" s="46" t="s">
+      <c r="AL4" s="46" t="s">
         <v>216</v>
       </c>
-      <c r="AL4" s="46" t="s">
+      <c r="AM4" s="46" t="s">
         <v>217</v>
       </c>
-      <c r="AM4" s="46" t="s">
+      <c r="AN4" s="46" t="s">
         <v>218</v>
       </c>
-      <c r="AN4" s="46" t="s">
+      <c r="AO4" s="46" t="s">
         <v>219</v>
       </c>
-      <c r="AO4" s="46" t="s">
+      <c r="AP4" s="46" t="s">
         <v>220</v>
       </c>
-      <c r="AP4" s="46" t="s">
+      <c r="AQ4" s="46" t="s">
         <v>221</v>
       </c>
-      <c r="AQ4" s="46" t="s">
+      <c r="AR4" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="AR4" s="46" t="s">
+      <c r="AS4" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="AS4" s="46" t="s">
+      <c r="AT4" s="46" t="s">
         <v>234</v>
       </c>
-      <c r="AT4" s="46" t="s">
+      <c r="AU4" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="AU4" s="46" t="s">
+      <c r="AV4" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="AV4" s="46" t="s">
+      <c r="AW4" s="46" t="s">
         <v>224</v>
       </c>
-      <c r="AW4" s="46" t="s">
+      <c r="AX4" s="46" t="s">
         <v>225</v>
       </c>
-      <c r="AX4" s="46" t="s">
+      <c r="AY4" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="AY4" s="46" t="s">
+      <c r="AZ4" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="AZ4" s="46" t="s">
+      <c r="BA4" s="46" t="s">
         <v>184</v>
       </c>
-      <c r="BA4" s="46" t="s">
+      <c r="BB4" s="46" t="s">
         <v>138</v>
       </c>
-      <c r="BB4" s="46" t="s">
+      <c r="BC4" s="46" t="s">
         <v>139</v>
       </c>
-      <c r="BC4" s="46" t="s">
+      <c r="BD4" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="BD4" s="46" t="s">
+      <c r="BE4" s="46" t="s">
         <v>185</v>
       </c>
-      <c r="BE4" s="46" t="s">
+      <c r="BF4" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="BF4" s="46" t="s">
+      <c r="BG4" s="46" t="s">
         <v>141</v>
       </c>
-      <c r="BG4" s="46" t="s">
+      <c r="BH4" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="BH4" s="46" t="s">
+      <c r="BI4" s="46" t="s">
         <v>57</v>
       </c>
-      <c r="BI4" s="46" t="s">
+      <c r="BJ4" s="46" t="s">
         <v>61</v>
       </c>
-      <c r="BJ4" s="49" t="s">
+      <c r="BK4" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="BK4" s="46" t="s">
+      <c r="BL4" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="BL4" s="46" t="s">
+      <c r="BM4" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="BM4" s="49" t="s">
+      <c r="BN4" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="BN4" s="49" t="s">
+      <c r="BO4" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="BO4" s="49" t="s">
+      <c r="BP4" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="BP4" s="49" t="s">
+      <c r="BQ4" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="BQ4" s="46" t="s">
+      <c r="BR4" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="BR4" s="46" t="s">
+      <c r="BS4" s="46" t="s">
         <v>130</v>
       </c>
-      <c r="BS4" s="46" t="s">
+      <c r="BT4" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="BT4" s="49" t="s">
+      <c r="BU4" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="BU4" s="46" t="s">
+      <c r="BV4" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="BV4" s="49" t="s">
+      <c r="BW4" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="BW4" s="46" t="s">
+      <c r="BX4" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="BX4" s="49" t="s">
+      <c r="BY4" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="BY4" s="49" t="s">
+      <c r="BZ4" s="49" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:77" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:78" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="41" t="s">
         <v>73</v>
       </c>
@@ -2403,170 +2421,173 @@
         <v>4</v>
       </c>
       <c r="X5" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="AA5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AC5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AD5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AF5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AM5" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AN5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AP5" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="AS5" s="4" t="s">
+      <c r="AT5" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="AT5" s="4" t="s">
+      <c r="AU5" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="AU5" s="4" t="s">
+      <c r="AV5" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="AV5" s="4" t="s">
+      <c r="AW5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AW5" s="4" t="s">
+      <c r="AX5" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="AX5" s="4" t="s">
+      <c r="AY5" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AZ5" s="4" t="s">
+      <c r="BA5" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="BA5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BC5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BD5" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="BD5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="BE5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="BF5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BH5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="BH5" s="4" t="s">
+      <c r="BI5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="BI5" s="4" t="s">
+      <c r="BJ5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BJ5" s="7" t="s">
+      <c r="BK5" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="BK5" s="4" t="s">
+      <c r="BL5" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="BM5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BM5" s="7" t="s">
+      <c r="BN5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BN5" s="45" t="s">
+      <c r="BO5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="BO5" s="7" t="s">
+      <c r="BP5" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="BP5" s="7" t="s">
+      <c r="BQ5" s="7" t="s">
         <v>162</v>
       </c>
-      <c r="BQ5" s="4" t="s">
+      <c r="BR5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="BR5" s="4" t="s">
+      <c r="BS5" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="BS5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="BT5" s="16" t="s">
+      <c r="BU5" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="BU5" s="4" t="s">
+      <c r="BV5" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="BV5" s="7" t="s">
+      <c r="BW5" s="7" t="s">
         <v>171</v>
       </c>
-      <c r="BW5" s="4" t="s">
+      <c r="BX5" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="BX5" s="7" t="s">
+      <c r="BY5" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="BY5" s="7" t="s">
+      <c r="BZ5" s="7" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="6" spans="1:77" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:77" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
       <c r="G7" s="38"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified Mapping comment; change required colors
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlf047\Documents\OldC\archivesspace\csvplugin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlf047\Documents\OldC\archivesspace\csvplugin\QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -125,9 +125,6 @@
     <t>Container information</t>
   </si>
   <si>
-    <t>box, drawer, etc.</t>
-  </si>
-  <si>
     <t>barcode</t>
   </si>
   <si>
@@ -745,6 +742,9 @@
   </si>
   <si>
     <t>Container Instance Type</t>
+  </si>
+  <si>
+    <t>A container type: box, drawer, etc.</t>
   </si>
 </sst>
 </file>
@@ -790,13 +790,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="5"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -853,6 +846,13 @@
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1058,13 +1058,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1082,10 +1076,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1122,25 +1116,25 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1187,8 +1181,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1569,16 +1569,16 @@
   <dimension ref="A1:ANZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="W3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X2" sqref="X2:X5"/>
+      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="37" customWidth="1"/>
-    <col min="2" max="2" width="16" style="21"/>
+    <col min="1" max="1" width="22.28515625" style="35" customWidth="1"/>
+    <col min="2" max="2" width="16" style="19"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
@@ -1586,7 +1586,7 @@
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="1"/>
     <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="54" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="52" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" style="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="1" customWidth="1"/>
@@ -1638,276 +1638,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
-        <v>235</v>
+      <c r="A1" s="35" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:78" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>108</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J2" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
+      </c>
+      <c r="J2" s="49" t="s">
+        <v>105</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L2" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="M2" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="N2" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="O2" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="P2" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q2" s="24" t="s">
-        <v>103</v>
+        <v>105</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="O2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="26" t="s">
+        <v>88</v>
+      </c>
+      <c r="X2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="26" t="s">
+      <c r="Y2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="27" t="s">
+      <c r="Z2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="27" t="s">
+      <c r="AA2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="27" t="s">
+      <c r="AB2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="27" t="s">
+      <c r="AC2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="27" t="s">
+      <c r="AD2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="27" t="s">
+      <c r="AE2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG2" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH2" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="AI2" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="AJ2" s="25" t="s">
+      <c r="AF2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AG2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AH2" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AK2" s="25" t="s">
+      <c r="AK2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="25" t="s">
+      <c r="AL2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AM2" s="25" t="s">
+      <c r="AM2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AN2" s="25" t="s">
+      <c r="AN2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="25" t="s">
+      <c r="AO2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AP2" s="25" t="s">
+      <c r="AP2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AQ2" s="25" t="s">
+      <c r="AQ2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AR2" s="25" t="s">
+      <c r="AR2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AS2" s="25" t="s">
+      <c r="AS2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="25" t="s">
+      <c r="AT2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AU2" s="25" t="s">
+      <c r="AU2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AV2" s="25" t="s">
+      <c r="AV2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AW2" s="25" t="s">
+      <c r="AW2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AX2" s="25" t="s">
+      <c r="AX2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AY2" s="25" t="s">
+      <c r="AY2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="AZ2" s="25" t="s">
+      <c r="AZ2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="BA2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BB2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BC2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BD2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BE2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BF2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BH2" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="BI2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BJ2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BK2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BL2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BM2" s="34" t="s">
-        <v>70</v>
-      </c>
-      <c r="BN2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BO2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BP2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BQ2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BR2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BS2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BT2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BU2" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="BV2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BW2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BX2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BY2" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="BZ2" s="35" t="s">
-        <v>70</v>
+      <c r="BA2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BB2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BD2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BE2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BF2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BH2" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="BI2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BJ2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BK2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BL2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BM2" s="32" t="s">
+        <v>69</v>
+      </c>
+      <c r="BN2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BO2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BP2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BQ2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BR2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BS2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BT2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BU2" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="BV2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BX2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BY2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="BZ2" s="33" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:78" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="40" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>105</v>
+      <c r="A3" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>104</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>113</v>
+        <v>71</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>112</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="J3" s="50" t="s">
         <v>181</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>182</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>2</v>
@@ -1922,16 +1922,16 @@
         <v>18</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S3" s="11" t="s">
         <v>22</v>
@@ -1940,452 +1940,452 @@
         <v>24</v>
       </c>
       <c r="U3" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="V3" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="W3" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" s="56" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y3" s="56" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z3" s="57" t="s">
+        <v>100</v>
+      </c>
+      <c r="AA3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB3" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AC3" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD3" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE3" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AF3" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG3" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="AH3" s="28" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI3" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="AJ3" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="AK3" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="AL3" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="AM3" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="AN3" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="AO3" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="AP3" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="AQ3" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="AR3" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS3" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="AT3" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="AU3" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV3" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="AW3" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="AX3" s="31" t="s">
+        <v>207</v>
+      </c>
+      <c r="AY3" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="AZ3" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="BA3" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="BB3" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="BC3" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="BD3" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="BE3" s="31" t="s">
+        <v>182</v>
+      </c>
+      <c r="BF3" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="BG3" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="BH3" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="BI3" s="30" t="s">
+        <v>153</v>
+      </c>
+      <c r="BJ3" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="BK3" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="BL3" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="BM3" s="30" t="s">
+        <v>157</v>
+      </c>
+      <c r="BN3" s="30" t="s">
+        <v>158</v>
+      </c>
+      <c r="BO3" s="30" t="s">
+        <v>159</v>
+      </c>
+      <c r="BP3" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="BQ3" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="BR3" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="BS3" s="30" t="s">
+        <v>165</v>
+      </c>
+      <c r="BT3" s="30" t="s">
+        <v>166</v>
+      </c>
+      <c r="BU3" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="BV3" s="30" t="s">
+        <v>168</v>
+      </c>
+      <c r="BW3" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="BX3" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="BY3" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="BZ3" s="30" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="1:78" s="48" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="40" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="44" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="44" t="s">
+        <v>133</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="K4" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="44" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="R4" s="44" t="s">
+        <v>89</v>
+      </c>
+      <c r="S4" s="44" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="44" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="V3" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="W3" s="43" t="s">
+      <c r="V4" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X4" s="44" t="s">
         <v>236</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Y4" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="Z3" s="15" t="s">
-        <v>101</v>
-      </c>
-      <c r="AA3" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AC3" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="AD3" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="AE3" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="AF3" s="30" t="s">
+      <c r="AB4" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="44" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="44" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="AG3" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="AH3" s="30" t="s">
-        <v>85</v>
-      </c>
-      <c r="AI3" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="AJ3" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="AK3" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="AL3" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="AM3" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="AN3" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="AO3" s="33" t="s">
-        <v>202</v>
-      </c>
-      <c r="AP3" s="33" t="s">
-        <v>204</v>
-      </c>
-      <c r="AQ3" s="33" t="s">
-        <v>201</v>
-      </c>
-      <c r="AR3" s="33" t="s">
-        <v>203</v>
-      </c>
-      <c r="AS3" s="33" t="s">
-        <v>205</v>
-      </c>
-      <c r="AT3" s="33" t="s">
-        <v>207</v>
-      </c>
-      <c r="AU3" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="AV3" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="AW3" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="AX3" s="33" t="s">
-        <v>208</v>
-      </c>
-      <c r="AY3" s="33" t="s">
-        <v>206</v>
-      </c>
-      <c r="AZ3" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="BA3" s="33" t="s">
+      <c r="AG4" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH4" s="44" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI4" s="44" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ4" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="AK4" s="44" t="s">
+        <v>214</v>
+      </c>
+      <c r="AL4" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="AM4" s="44" t="s">
+        <v>216</v>
+      </c>
+      <c r="AN4" s="44" t="s">
+        <v>217</v>
+      </c>
+      <c r="AO4" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="AP4" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="AQ4" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="AR4" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="AS4" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="AT4" s="44" t="s">
+        <v>233</v>
+      </c>
+      <c r="AU4" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="AV4" s="44" t="s">
+        <v>222</v>
+      </c>
+      <c r="AW4" s="44" t="s">
+        <v>223</v>
+      </c>
+      <c r="AX4" s="44" t="s">
+        <v>224</v>
+      </c>
+      <c r="AY4" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="AZ4" s="44" t="s">
+        <v>225</v>
+      </c>
+      <c r="BA4" s="44" t="s">
         <v>183</v>
       </c>
-      <c r="BB3" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="BC3" s="33" t="s">
+      <c r="BB4" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="BD3" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="BE3" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="BF3" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="BG3" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="BH3" s="33" t="s">
-        <v>213</v>
-      </c>
-      <c r="BI3" s="32" t="s">
-        <v>154</v>
-      </c>
-      <c r="BJ3" s="32" t="s">
-        <v>155</v>
-      </c>
-      <c r="BK3" s="32" t="s">
-        <v>156</v>
-      </c>
-      <c r="BL3" s="32" t="s">
-        <v>157</v>
-      </c>
-      <c r="BM3" s="32" t="s">
-        <v>158</v>
-      </c>
-      <c r="BN3" s="32" t="s">
-        <v>159</v>
-      </c>
-      <c r="BO3" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="BP3" s="32" t="s">
-        <v>161</v>
-      </c>
-      <c r="BQ3" s="32" t="s">
-        <v>163</v>
-      </c>
-      <c r="BR3" s="32" t="s">
-        <v>164</v>
-      </c>
-      <c r="BS3" s="32" t="s">
-        <v>166</v>
-      </c>
-      <c r="BT3" s="32" t="s">
-        <v>167</v>
-      </c>
-      <c r="BU3" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="BV3" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="BW3" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="BX3" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="BY3" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="BZ3" s="32" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="4" spans="1:78" s="50" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="42" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="47" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="46" t="s">
-        <v>55</v>
-      </c>
-      <c r="D4" s="48" t="s">
-        <v>76</v>
-      </c>
-      <c r="E4" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="G4" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="H4" s="46" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="J4" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="K4" s="46" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="46" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="46" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="46" t="s">
-        <v>81</v>
-      </c>
-      <c r="R4" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="S4" s="46" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="46" t="s">
-        <v>14</v>
-      </c>
-      <c r="U4" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="V4" s="46" t="s">
-        <v>42</v>
-      </c>
-      <c r="W4" s="49" t="s">
-        <v>41</v>
-      </c>
-      <c r="X4" s="46" t="s">
-        <v>237</v>
-      </c>
-      <c r="Y4" s="46" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z4" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="46" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB4" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC4" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD4" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE4" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="AF4" s="46" t="s">
-        <v>84</v>
-      </c>
-      <c r="AG4" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="AH4" s="46" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI4" s="46" t="s">
-        <v>231</v>
-      </c>
-      <c r="AJ4" s="46" t="s">
-        <v>214</v>
-      </c>
-      <c r="AK4" s="46" t="s">
-        <v>215</v>
-      </c>
-      <c r="AL4" s="46" t="s">
-        <v>216</v>
-      </c>
-      <c r="AM4" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="AN4" s="46" t="s">
-        <v>218</v>
-      </c>
-      <c r="AO4" s="46" t="s">
-        <v>219</v>
-      </c>
-      <c r="AP4" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="AQ4" s="46" t="s">
-        <v>221</v>
-      </c>
-      <c r="AR4" s="46" t="s">
-        <v>232</v>
-      </c>
-      <c r="AS4" s="46" t="s">
-        <v>233</v>
-      </c>
-      <c r="AT4" s="46" t="s">
-        <v>234</v>
-      </c>
-      <c r="AU4" s="46" t="s">
-        <v>222</v>
-      </c>
-      <c r="AV4" s="46" t="s">
-        <v>223</v>
-      </c>
-      <c r="AW4" s="46" t="s">
-        <v>224</v>
-      </c>
-      <c r="AX4" s="46" t="s">
-        <v>225</v>
-      </c>
-      <c r="AY4" s="46" t="s">
-        <v>227</v>
-      </c>
-      <c r="AZ4" s="46" t="s">
-        <v>226</v>
-      </c>
-      <c r="BA4" s="46" t="s">
+      <c r="BC4" s="44" t="s">
+        <v>138</v>
+      </c>
+      <c r="BD4" s="44" t="s">
+        <v>185</v>
+      </c>
+      <c r="BE4" s="44" t="s">
         <v>184</v>
       </c>
-      <c r="BB4" s="46" t="s">
-        <v>138</v>
-      </c>
-      <c r="BC4" s="46" t="s">
+      <c r="BF4" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="BD4" s="46" t="s">
+      <c r="BG4" s="44" t="s">
+        <v>140</v>
+      </c>
+      <c r="BH4" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="BE4" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="BF4" s="46" t="s">
-        <v>140</v>
-      </c>
-      <c r="BG4" s="46" t="s">
-        <v>141</v>
-      </c>
-      <c r="BH4" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="BI4" s="46" t="s">
+      <c r="BI4" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="BJ4" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="BK4" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="BL4" s="44" t="s">
+        <v>58</v>
+      </c>
+      <c r="BM4" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="BN4" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="BO4" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="BP4" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ4" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR4" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="BS4" s="44" t="s">
+        <v>129</v>
+      </c>
+      <c r="BT4" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="BU4" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="BV4" s="44" t="s">
         <v>57</v>
       </c>
-      <c r="BJ4" s="46" t="s">
-        <v>61</v>
-      </c>
-      <c r="BK4" s="49" t="s">
-        <v>64</v>
-      </c>
-      <c r="BL4" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM4" s="46" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN4" s="49" t="s">
-        <v>63</v>
-      </c>
-      <c r="BO4" s="49" t="s">
-        <v>129</v>
-      </c>
-      <c r="BP4" s="49" t="s">
+      <c r="BW4" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="BX4" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="BY4" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="BQ4" s="49" t="s">
+      <c r="BZ4" s="47" t="s">
         <v>65</v>
-      </c>
-      <c r="BR4" s="46" t="s">
-        <v>62</v>
-      </c>
-      <c r="BS4" s="46" t="s">
-        <v>130</v>
-      </c>
-      <c r="BT4" s="46" t="s">
-        <v>131</v>
-      </c>
-      <c r="BU4" s="49" t="s">
-        <v>95</v>
-      </c>
-      <c r="BV4" s="46" t="s">
-        <v>58</v>
-      </c>
-      <c r="BW4" s="49" t="s">
-        <v>69</v>
-      </c>
-      <c r="BX4" s="46" t="s">
-        <v>94</v>
-      </c>
-      <c r="BY4" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="BZ4" s="49" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:78" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>104</v>
+      <c r="A5" s="39" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" s="18" t="s">
+        <v>103</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="22" t="s">
-        <v>110</v>
+      <c r="F5" s="20" t="s">
+        <v>109</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="J5" s="53" t="s">
         <v>178</v>
-      </c>
-      <c r="J5" s="55" t="s">
-        <v>179</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>28</v>
@@ -2400,10 +2400,10 @@
         <v>19</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>22</v>
@@ -2412,183 +2412,183 @@
         <v>31</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="W5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="Y5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="Z5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="AA5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AB5" s="4" t="s">
-        <v>36</v>
-      </c>
       <c r="AC5" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AE5" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AD5" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AE5" s="4" t="s">
-        <v>98</v>
-      </c>
       <c r="AF5" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AG5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK5" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL5" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="AM5" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN5" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AO5" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AP5" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AQ5" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR5" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="AS5" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="AT5" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="AU5" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="AV5" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="AW5" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="AX5" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="AY5" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="AZ5" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="BA5" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BF5" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BG5" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="BH5" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="BI5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="BJ5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="BK5" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="BL5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="BM5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AI5" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="AJ5" s="4" t="s">
-        <v>193</v>
-      </c>
-      <c r="AK5" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="AL5" s="4" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM5" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN5" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO5" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="AP5" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="AQ5" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR5" s="4" t="s">
-        <v>203</v>
-      </c>
-      <c r="AS5" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="AT5" s="4" t="s">
-        <v>211</v>
-      </c>
-      <c r="AU5" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>212</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="AX5" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AY5" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="AZ5" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="BA5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="BB5" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="BC5" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="BD5" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="BG5" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="BH5" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="BI5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BN5" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="BO5" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="BP5" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="BQ5" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="BR5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BK5" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="BL5" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="BM5" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="BN5" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="BO5" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="BP5" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="BQ5" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="BR5" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="BS5" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="BT5" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="BU5" s="16" t="s">
-        <v>96</v>
+        <v>131</v>
+      </c>
+      <c r="BU5" s="14" t="s">
+        <v>95</v>
       </c>
       <c r="BV5" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="BW5" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="BX5" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="BY5" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BZ5" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="G7" s="38"/>
+      <c r="G7" s="36"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2629,43 +2629,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
-        <v>115</v>
+      <c r="A1" s="21" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="56" t="s">
-        <v>152</v>
+      <c r="A7" s="54" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -2682,43 +2682,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142" style="44" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="142" style="42" bestFit="1" customWidth="1"/>
     <col min="2" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="44" t="s">
-        <v>126</v>
+      <c r="A1" s="42" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="44" t="s">
-        <v>125</v>
+      <c r="A3" s="42" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
-        <v>114</v>
+      <c r="A4" s="42" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="44" t="s">
-        <v>122</v>
+      <c r="A5" s="42" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="44" t="s">
-        <v>121</v>
+      <c r="A6" s="42" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
-        <v>123</v>
+      <c r="A7" s="42" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="44" t="s">
-        <v>124</v>
+      <c r="A8" s="42" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
make indicator_ columns "text" instead of "general"
Resolves issue #6 (https://github.com/harvard-library/aspace-import-excel/issues/6 )
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlf047\Documents\OldC\archivesspace\csvplugin\QA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlf047\Documents\OldC\archivesspace\csvplugin\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1017,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1188,7 +1188,19 @@
     <xf numFmtId="0" fontId="14" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1569,10 +1581,10 @@
   <dimension ref="A1:ANZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z3" sqref="Z3"/>
+      <selection pane="bottomRight" activeCell="AE1" sqref="AE1:AE1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,12 +1606,13 @@
     <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="24" width="26.85546875" style="1" customWidth="1"/>
-    <col min="25" max="26" width="23" style="1"/>
+    <col min="25" max="25" width="23" style="1"/>
+    <col min="26" max="26" width="23" style="57"/>
     <col min="27" max="27" width="10.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="1" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="19" style="57" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" style="57" customWidth="1"/>
     <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="1" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="57" customWidth="1"/>
     <col min="32" max="32" width="10.42578125" style="1" customWidth="1"/>
     <col min="33" max="34" width="9.140625" style="1"/>
     <col min="35" max="35" width="15.28515625" style="1" customWidth="1"/>
@@ -1718,22 +1731,22 @@
       <c r="Y2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="25" t="s">
+      <c r="Z2" s="58" t="s">
         <v>33</v>
       </c>
       <c r="AA2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="25" t="s">
+      <c r="AB2" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="25" t="s">
+      <c r="AC2" s="58" t="s">
         <v>33</v>
       </c>
       <c r="AD2" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="25" t="s">
+      <c r="AE2" s="58" t="s">
         <v>33</v>
       </c>
       <c r="AF2" s="26" t="s">
@@ -1954,22 +1967,22 @@
       <c r="Y3" s="56" t="s">
         <v>238</v>
       </c>
-      <c r="Z3" s="57" t="s">
+      <c r="Z3" s="61" t="s">
         <v>100</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AB3" s="59" t="s">
         <v>90</v>
       </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AC3" s="59" t="s">
         <v>98</v>
       </c>
       <c r="AD3" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="AE3" s="13" t="s">
+      <c r="AE3" s="59" t="s">
         <v>99</v>
       </c>
       <c r="AF3" s="28" t="s">
@@ -2190,22 +2203,22 @@
       <c r="Y4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="Z4" s="44" t="s">
+      <c r="Z4" s="46" t="s">
         <v>10</v>
       </c>
       <c r="AA4" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="44" t="s">
+      <c r="AB4" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="44" t="s">
+      <c r="AC4" s="46" t="s">
         <v>12</v>
       </c>
       <c r="AD4" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="AE4" s="44" t="s">
+      <c r="AE4" s="46" t="s">
         <v>37</v>
       </c>
       <c r="AF4" s="44" t="s">
@@ -2426,22 +2439,22 @@
       <c r="Y5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="4" t="s">
+      <c r="Z5" s="60" t="s">
         <v>101</v>
       </c>
       <c r="AA5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="4" t="s">
+      <c r="AB5" s="60" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="4" t="s">
+      <c r="AC5" s="60" t="s">
         <v>96</v>
       </c>
       <c r="AD5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AE5" s="4" t="s">
+      <c r="AE5" s="60" t="s">
         <v>97</v>
       </c>
       <c r="AF5" s="4" t="s">

</xml_diff>

<commit_message>
changed date formats from general to text
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18750" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="7860"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1017,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1201,6 +1201,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="14" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1581,10 +1587,10 @@
   <dimension ref="A1:ANZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AE1" sqref="AE1:AE1048576"/>
+      <selection pane="bottomRight" activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,8 +1607,8 @@
     <col min="10" max="10" width="13.5703125" style="52" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="11" style="57" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="57" customWidth="1"/>
     <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="24" width="26.85546875" style="1" customWidth="1"/>
@@ -1692,10 +1698,10 @@
       <c r="L2" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="62" t="s">
         <v>102</v>
       </c>
-      <c r="N2" s="22" t="s">
+      <c r="N2" s="62" t="s">
         <v>102</v>
       </c>
       <c r="O2" s="22" t="s">
@@ -1928,10 +1934,10 @@
       <c r="L3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="63" t="s">
         <v>18</v>
       </c>
       <c r="O3" s="9" t="s">
@@ -2164,10 +2170,10 @@
       <c r="L4" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="M4" s="44" t="s">
+      <c r="M4" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="44" t="s">
+      <c r="N4" s="46" t="s">
         <v>27</v>
       </c>
       <c r="O4" s="44" t="s">
@@ -2400,10 +2406,10 @@
       <c r="L5" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="M5" s="4" t="s">
+      <c r="M5" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="60" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="6" t="s">

</xml_diff>

<commit_message>
"hide" resource identifier field, clean up eadid
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18720" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -236,9 +236,6 @@
     <t>Processing Information</t>
   </si>
   <si>
-    <t>EAD ID (if defining the Resource)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Field name </t>
   </si>
   <si>
@@ -745,13 +742,16 @@
   </si>
   <si>
     <t>A container type: box, drawer, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EAD ID </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -853,6 +853,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1070,9 +1077,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1207,6 +1211,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1587,16 +1594,16 @@
   <dimension ref="A1:ANZ7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N1" sqref="N1:N1048576"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="35" customWidth="1"/>
-    <col min="2" max="2" width="16" style="19"/>
+    <col min="1" max="1" width="22.28515625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="0" style="18" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
@@ -1604,21 +1611,21 @@
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="1"/>
     <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="52" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" style="51" customWidth="1"/>
     <col min="11" max="11" width="24" style="1" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="57" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="57" customWidth="1"/>
+    <col min="13" max="13" width="11" style="56" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="56" customWidth="1"/>
     <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
     <col min="17" max="24" width="26.85546875" style="1" customWidth="1"/>
     <col min="25" max="25" width="23" style="1"/>
-    <col min="26" max="26" width="23" style="57"/>
+    <col min="26" max="26" width="23" style="56"/>
     <col min="27" max="27" width="10.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="57" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" style="57" customWidth="1"/>
+    <col min="28" max="28" width="19" style="56" customWidth="1"/>
+    <col min="29" max="29" width="19.140625" style="56" customWidth="1"/>
     <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="57" customWidth="1"/>
+    <col min="31" max="31" width="11.42578125" style="56" customWidth="1"/>
     <col min="32" max="32" width="10.42578125" style="1" customWidth="1"/>
     <col min="33" max="34" width="9.140625" style="1"/>
     <col min="35" max="35" width="15.28515625" style="1" customWidth="1"/>
@@ -1657,276 +1664,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>234</v>
+      <c r="A1" s="34" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:78" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>106</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="J2" s="49" t="s">
-        <v>105</v>
+        <v>104</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>104</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="M2" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="N2" s="62" t="s">
-        <v>102</v>
-      </c>
-      <c r="O2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="Q2" s="22" t="s">
-        <v>102</v>
+        <v>104</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="M2" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="N2" s="61" t="s">
+        <v>101</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="X2" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="Y2" s="24" t="s">
+      <c r="Y2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="58" t="s">
+      <c r="Z2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="25" t="s">
+      <c r="AA2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="58" t="s">
+      <c r="AB2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AC2" s="58" t="s">
+      <c r="AC2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="25" t="s">
+      <c r="AD2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="58" t="s">
+      <c r="AE2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="26" t="s">
+      <c r="AF2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AG2" s="26" t="s">
+      <c r="AG2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="27" t="s">
+      <c r="AH2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="55" t="s">
-        <v>92</v>
-      </c>
-      <c r="AJ2" s="23" t="s">
+      <c r="AI2" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AK2" s="23" t="s">
+      <c r="AK2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AL2" s="23" t="s">
+      <c r="AL2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AM2" s="23" t="s">
+      <c r="AM2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AN2" s="23" t="s">
+      <c r="AN2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AO2" s="23" t="s">
+      <c r="AO2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AP2" s="23" t="s">
+      <c r="AP2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AQ2" s="23" t="s">
+      <c r="AQ2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AR2" s="23" t="s">
+      <c r="AR2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AS2" s="23" t="s">
+      <c r="AS2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AT2" s="23" t="s">
+      <c r="AT2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AU2" s="23" t="s">
+      <c r="AU2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AV2" s="23" t="s">
+      <c r="AV2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AW2" s="23" t="s">
+      <c r="AW2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AX2" s="23" t="s">
+      <c r="AX2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AY2" s="23" t="s">
+      <c r="AY2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="AZ2" s="23" t="s">
+      <c r="AZ2" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="BA2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BB2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BC2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BD2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BE2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BF2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BG2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BH2" s="23" t="s">
-        <v>134</v>
-      </c>
-      <c r="BI2" s="33" t="s">
+      <c r="BA2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BB2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BC2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BD2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BF2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BG2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BH2" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="BI2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BJ2" s="33" t="s">
+      <c r="BJ2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BK2" s="33" t="s">
+      <c r="BK2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BL2" s="33" t="s">
+      <c r="BL2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BM2" s="32" t="s">
+      <c r="BM2" s="31" t="s">
         <v>69</v>
       </c>
-      <c r="BN2" s="33" t="s">
+      <c r="BN2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BO2" s="33" t="s">
+      <c r="BO2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BP2" s="33" t="s">
+      <c r="BP2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BQ2" s="33" t="s">
+      <c r="BQ2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BR2" s="33" t="s">
+      <c r="BR2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BS2" s="33" t="s">
+      <c r="BS2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BT2" s="33" t="s">
+      <c r="BT2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BU2" s="34" t="s">
+      <c r="BU2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="BV2" s="33" t="s">
+      <c r="BV2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BW2" s="33" t="s">
+      <c r="BW2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BX2" s="33" t="s">
+      <c r="BX2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BY2" s="33" t="s">
+      <c r="BY2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BZ2" s="33" t="s">
+      <c r="BZ2" s="32" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:78" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="38" t="s">
-        <v>73</v>
+      <c r="A3" s="37" t="s">
+        <v>72</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>71</v>
+        <v>238</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G3" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J3" s="49" t="s">
         <v>180</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="J3" s="50" t="s">
-        <v>181</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>2</v>
@@ -1934,23 +1941,23 @@
       <c r="L3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="63" t="s">
+      <c r="M3" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="63" t="s">
+      <c r="N3" s="62" t="s">
         <v>18</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="R3" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="S3" s="11" t="s">
         <v>22</v>
@@ -1959,457 +1966,457 @@
         <v>24</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="W3" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="W3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="56" t="s">
-        <v>235</v>
-      </c>
-      <c r="Y3" s="56" t="s">
-        <v>238</v>
-      </c>
-      <c r="Z3" s="61" t="s">
-        <v>100</v>
+      <c r="X3" s="55" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y3" s="55" t="s">
+        <v>237</v>
+      </c>
+      <c r="Z3" s="60" t="s">
+        <v>99</v>
       </c>
       <c r="AA3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="59" t="s">
+      <c r="AB3" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC3" s="58" t="s">
+        <v>97</v>
+      </c>
+      <c r="AD3" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="AC3" s="59" t="s">
+      <c r="AE3" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="AD3" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE3" s="59" t="s">
-        <v>99</v>
-      </c>
-      <c r="AF3" s="28" t="s">
+      <c r="AF3" s="27" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG3" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="AH3" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="AI3" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="AJ3" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="AK3" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="AL3" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="AM3" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="AN3" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO3" s="30" t="s">
+        <v>200</v>
+      </c>
+      <c r="AP3" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="AQ3" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="AR3" s="30" t="s">
+        <v>201</v>
+      </c>
+      <c r="AS3" s="30" t="s">
+        <v>203</v>
+      </c>
+      <c r="AT3" s="30" t="s">
+        <v>205</v>
+      </c>
+      <c r="AU3" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="AV3" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="AW3" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="AX3" s="30" t="s">
+        <v>206</v>
+      </c>
+      <c r="AY3" s="30" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ3" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="BA3" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="BB3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="BC3" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="BD3" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="BE3" s="30" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="BG3" s="30" t="s">
+        <v>135</v>
+      </c>
+      <c r="BH3" s="30" t="s">
+        <v>211</v>
+      </c>
+      <c r="BI3" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="BJ3" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="BK3" s="29" t="s">
+        <v>154</v>
+      </c>
+      <c r="BL3" s="29" t="s">
+        <v>155</v>
+      </c>
+      <c r="BM3" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="BN3" s="29" t="s">
+        <v>157</v>
+      </c>
+      <c r="BO3" s="29" t="s">
+        <v>158</v>
+      </c>
+      <c r="BP3" s="29" t="s">
+        <v>159</v>
+      </c>
+      <c r="BQ3" s="29" t="s">
+        <v>161</v>
+      </c>
+      <c r="BR3" s="29" t="s">
+        <v>162</v>
+      </c>
+      <c r="BS3" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="BT3" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="BU3" s="29" t="s">
+        <v>166</v>
+      </c>
+      <c r="BV3" s="29" t="s">
+        <v>167</v>
+      </c>
+      <c r="BW3" s="29" t="s">
+        <v>168</v>
+      </c>
+      <c r="BX3" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="BY3" s="29" t="s">
+        <v>172</v>
+      </c>
+      <c r="BZ3" s="29" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="4" spans="1:78" s="47" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H4" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="J4" s="50" t="s">
+        <v>144</v>
+      </c>
+      <c r="K4" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="N4" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="O4" s="43" t="s">
+        <v>21</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q4" s="43" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="S4" s="43" t="s">
+        <v>23</v>
+      </c>
+      <c r="T4" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="U4" s="43" t="s">
+        <v>146</v>
+      </c>
+      <c r="V4" s="43" t="s">
+        <v>41</v>
+      </c>
+      <c r="W4" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="X4" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y4" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z4" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA4" s="43" t="s">
+        <v>34</v>
+      </c>
+      <c r="AB4" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="AC4" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" s="43" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE4" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="AF4" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="AG3" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="AH3" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="AI3" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="AJ3" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="AK3" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="AL3" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="AM3" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="AN3" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="AO3" s="31" t="s">
-        <v>201</v>
-      </c>
-      <c r="AP3" s="31" t="s">
-        <v>203</v>
-      </c>
-      <c r="AQ3" s="31" t="s">
-        <v>200</v>
-      </c>
-      <c r="AR3" s="31" t="s">
-        <v>202</v>
-      </c>
-      <c r="AS3" s="31" t="s">
-        <v>204</v>
-      </c>
-      <c r="AT3" s="31" t="s">
-        <v>206</v>
-      </c>
-      <c r="AU3" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV3" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="AW3" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="AX3" s="31" t="s">
-        <v>207</v>
-      </c>
-      <c r="AY3" s="31" t="s">
-        <v>205</v>
-      </c>
-      <c r="AZ3" s="31" t="s">
-        <v>208</v>
-      </c>
-      <c r="BA3" s="31" t="s">
+      <c r="AG4" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH4" s="43" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI4" s="43" t="s">
+        <v>229</v>
+      </c>
+      <c r="AJ4" s="43" t="s">
+        <v>212</v>
+      </c>
+      <c r="AK4" s="43" t="s">
+        <v>213</v>
+      </c>
+      <c r="AL4" s="43" t="s">
+        <v>214</v>
+      </c>
+      <c r="AM4" s="43" t="s">
+        <v>215</v>
+      </c>
+      <c r="AN4" s="43" t="s">
+        <v>216</v>
+      </c>
+      <c r="AO4" s="43" t="s">
+        <v>217</v>
+      </c>
+      <c r="AP4" s="43" t="s">
+        <v>218</v>
+      </c>
+      <c r="AQ4" s="43" t="s">
+        <v>219</v>
+      </c>
+      <c r="AR4" s="43" t="s">
+        <v>230</v>
+      </c>
+      <c r="AS4" s="43" t="s">
+        <v>231</v>
+      </c>
+      <c r="AT4" s="43" t="s">
+        <v>232</v>
+      </c>
+      <c r="AU4" s="43" t="s">
+        <v>220</v>
+      </c>
+      <c r="AV4" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="AW4" s="43" t="s">
+        <v>222</v>
+      </c>
+      <c r="AX4" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="AY4" s="43" t="s">
+        <v>225</v>
+      </c>
+      <c r="AZ4" s="43" t="s">
+        <v>224</v>
+      </c>
+      <c r="BA4" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="BB3" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="BC3" s="31" t="s">
+      <c r="BB4" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="BD3" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="BE3" s="31" t="s">
-        <v>182</v>
-      </c>
-      <c r="BF3" s="31" t="s">
-        <v>135</v>
-      </c>
-      <c r="BG3" s="31" t="s">
-        <v>136</v>
-      </c>
-      <c r="BH3" s="31" t="s">
-        <v>212</v>
-      </c>
-      <c r="BI3" s="30" t="s">
-        <v>153</v>
-      </c>
-      <c r="BJ3" s="30" t="s">
-        <v>154</v>
-      </c>
-      <c r="BK3" s="30" t="s">
-        <v>155</v>
-      </c>
-      <c r="BL3" s="30" t="s">
-        <v>156</v>
-      </c>
-      <c r="BM3" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="BN3" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="BO3" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="BP3" s="30" t="s">
-        <v>160</v>
-      </c>
-      <c r="BQ3" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="BR3" s="30" t="s">
-        <v>163</v>
-      </c>
-      <c r="BS3" s="30" t="s">
-        <v>165</v>
-      </c>
-      <c r="BT3" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="BU3" s="30" t="s">
-        <v>167</v>
-      </c>
-      <c r="BV3" s="30" t="s">
-        <v>168</v>
-      </c>
-      <c r="BW3" s="30" t="s">
-        <v>169</v>
-      </c>
-      <c r="BX3" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="BY3" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="BZ3" s="30" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="4" spans="1:78" s="48" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="45" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="D4" s="46" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="44" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="47" t="s">
-        <v>110</v>
-      </c>
-      <c r="G4" s="44" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="44" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="44" t="s">
-        <v>133</v>
-      </c>
-      <c r="J4" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="K4" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" s="44" t="s">
-        <v>78</v>
-      </c>
-      <c r="M4" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="N4" s="46" t="s">
-        <v>27</v>
-      </c>
-      <c r="O4" s="44" t="s">
-        <v>21</v>
-      </c>
-      <c r="P4" s="44" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" s="44" t="s">
-        <v>80</v>
-      </c>
-      <c r="R4" s="44" t="s">
-        <v>89</v>
-      </c>
-      <c r="S4" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="T4" s="44" t="s">
-        <v>14</v>
-      </c>
-      <c r="U4" s="44" t="s">
-        <v>147</v>
-      </c>
-      <c r="V4" s="44" t="s">
-        <v>41</v>
-      </c>
-      <c r="W4" s="47" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" s="44" t="s">
-        <v>236</v>
-      </c>
-      <c r="Y4" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="Z4" s="46" t="s">
-        <v>10</v>
-      </c>
-      <c r="AA4" s="44" t="s">
-        <v>34</v>
-      </c>
-      <c r="AB4" s="46" t="s">
-        <v>11</v>
-      </c>
-      <c r="AC4" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="AD4" s="44" t="s">
-        <v>36</v>
-      </c>
-      <c r="AE4" s="46" t="s">
-        <v>37</v>
-      </c>
-      <c r="AF4" s="44" t="s">
-        <v>83</v>
-      </c>
-      <c r="AG4" s="44" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH4" s="44" t="s">
-        <v>46</v>
-      </c>
-      <c r="AI4" s="44" t="s">
-        <v>230</v>
-      </c>
-      <c r="AJ4" s="44" t="s">
-        <v>213</v>
-      </c>
-      <c r="AK4" s="44" t="s">
-        <v>214</v>
-      </c>
-      <c r="AL4" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="AM4" s="44" t="s">
-        <v>216</v>
-      </c>
-      <c r="AN4" s="44" t="s">
-        <v>217</v>
-      </c>
-      <c r="AO4" s="44" t="s">
-        <v>218</v>
-      </c>
-      <c r="AP4" s="44" t="s">
-        <v>219</v>
-      </c>
-      <c r="AQ4" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="AR4" s="44" t="s">
-        <v>231</v>
-      </c>
-      <c r="AS4" s="44" t="s">
-        <v>232</v>
-      </c>
-      <c r="AT4" s="44" t="s">
-        <v>233</v>
-      </c>
-      <c r="AU4" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="AV4" s="44" t="s">
-        <v>222</v>
-      </c>
-      <c r="AW4" s="44" t="s">
-        <v>223</v>
-      </c>
-      <c r="AX4" s="44" t="s">
-        <v>224</v>
-      </c>
-      <c r="AY4" s="44" t="s">
-        <v>226</v>
-      </c>
-      <c r="AZ4" s="44" t="s">
-        <v>225</v>
-      </c>
-      <c r="BA4" s="44" t="s">
+      <c r="BC4" s="43" t="s">
+        <v>137</v>
+      </c>
+      <c r="BD4" s="43" t="s">
+        <v>184</v>
+      </c>
+      <c r="BE4" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="BB4" s="44" t="s">
-        <v>137</v>
-      </c>
-      <c r="BC4" s="44" t="s">
+      <c r="BF4" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="BD4" s="44" t="s">
+      <c r="BG4" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="BH4" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="BE4" s="44" t="s">
-        <v>184</v>
-      </c>
-      <c r="BF4" s="44" t="s">
-        <v>139</v>
-      </c>
-      <c r="BG4" s="44" t="s">
-        <v>140</v>
-      </c>
-      <c r="BH4" s="44" t="s">
-        <v>186</v>
-      </c>
-      <c r="BI4" s="44" t="s">
+      <c r="BI4" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="BJ4" s="44" t="s">
+      <c r="BJ4" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="BK4" s="47" t="s">
+      <c r="BK4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="BL4" s="44" t="s">
+      <c r="BL4" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BM4" s="44" t="s">
+      <c r="BM4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="BN4" s="47" t="s">
+      <c r="BN4" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="BO4" s="47" t="s">
+      <c r="BO4" s="46" t="s">
+        <v>127</v>
+      </c>
+      <c r="BP4" s="46" t="s">
+        <v>66</v>
+      </c>
+      <c r="BQ4" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="BR4" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="BS4" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="BP4" s="47" t="s">
-        <v>66</v>
-      </c>
-      <c r="BQ4" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR4" s="44" t="s">
-        <v>61</v>
-      </c>
-      <c r="BS4" s="44" t="s">
+      <c r="BT4" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="BT4" s="44" t="s">
-        <v>130</v>
-      </c>
-      <c r="BU4" s="47" t="s">
-        <v>94</v>
-      </c>
-      <c r="BV4" s="44" t="s">
+      <c r="BU4" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="BV4" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BW4" s="47" t="s">
+      <c r="BW4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="BX4" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="BY4" s="47" t="s">
+      <c r="BX4" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="BZ4" s="47" t="s">
+      <c r="BZ4" s="46" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:78" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>103</v>
+      <c r="A5" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="63" t="s">
+        <v>102</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="20" t="s">
-        <v>109</v>
+      <c r="F5" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="J5" s="52" t="s">
         <v>177</v>
-      </c>
-      <c r="J5" s="53" t="s">
-        <v>178</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="M5" s="60" t="s">
+        <v>178</v>
+      </c>
+      <c r="M5" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="60" t="s">
+      <c r="N5" s="59" t="s">
         <v>29</v>
       </c>
       <c r="O5" s="6" t="s">
@@ -2419,10 +2426,10 @@
         <v>19</v>
       </c>
       <c r="Q5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>22</v>
@@ -2431,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="U5" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="V5" s="4" t="s">
         <v>55</v>
@@ -2440,31 +2447,31 @@
         <v>4</v>
       </c>
       <c r="X5" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="Y5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="60" t="s">
-        <v>101</v>
+      <c r="Z5" s="59" t="s">
+        <v>100</v>
       </c>
       <c r="AA5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="60" t="s">
+      <c r="AB5" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="60" t="s">
-        <v>96</v>
+      <c r="AC5" s="59" t="s">
+        <v>95</v>
       </c>
       <c r="AD5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AE5" s="60" t="s">
-        <v>97</v>
+      <c r="AE5" s="59" t="s">
+        <v>96</v>
       </c>
       <c r="AF5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AG5" s="4" t="s">
         <v>47</v>
@@ -2473,82 +2480,82 @@
         <v>48</v>
       </c>
       <c r="AI5" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ5" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AM5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="AN5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AP5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AQ5" s="4" t="s">
-        <v>199</v>
-      </c>
       <c r="AR5" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="AS5" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="AT5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="AT5" s="4" t="s">
+      <c r="AU5" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="AV5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="AU5" s="4" t="s">
-        <v>207</v>
-      </c>
-      <c r="AV5" s="4" t="s">
-        <v>211</v>
-      </c>
       <c r="AW5" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="AX5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="AX5" s="4" t="s">
+      <c r="AY5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AY5" s="4" t="s">
-        <v>229</v>
-      </c>
       <c r="AZ5" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="BA5" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="BB5" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="BE5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="BB5" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BD5" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="BE5" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="BF5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BG5" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="BH5" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BI5" s="4" t="s">
         <v>42</v>
@@ -2560,7 +2567,7 @@
         <v>53</v>
       </c>
       <c r="BL5" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BM5" s="4" t="s">
         <v>49</v>
@@ -2568,46 +2575,46 @@
       <c r="BN5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BO5" s="43" t="s">
+      <c r="BO5" s="42" t="s">
         <v>4</v>
       </c>
       <c r="BP5" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="BQ5" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="BR5" s="4" t="s">
         <v>51</v>
       </c>
       <c r="BS5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BT5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="BU5" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="BV5" s="4" t="s">
         <v>70</v>
       </c>
       <c r="BW5" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="BX5" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="BY5" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BZ5" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="6" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="G7" s="36"/>
+      <c r="G7" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="5">
@@ -2648,43 +2655,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>114</v>
+      <c r="A1" s="20" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
-        <v>151</v>
+      <c r="A7" s="53" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -2701,43 +2708,43 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142" style="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="142" style="41" bestFit="1" customWidth="1"/>
     <col min="2" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
-        <v>125</v>
+      <c r="A1" s="41" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>124</v>
+      <c r="A3" s="41" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
-        <v>113</v>
+      <c r="A4" s="41" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="42" t="s">
-        <v>121</v>
+      <c r="A5" s="41" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>120</v>
+      <c r="A6" s="41" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>122</v>
+      <c r="A7" s="41" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
-        <v>123</v>
+      <c r="A8" s="41" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support 'Other Level' as a Description Level selection
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="241">
   <si>
     <t>Mapping - ArchivesSpace Resource record SECTION</t>
   </si>
@@ -745,6 +745,12 @@
   </si>
   <si>
     <t xml:space="preserve">EAD ID </t>
+  </si>
+  <si>
+    <t>other_level</t>
+  </si>
+  <si>
+    <t>Other Level</t>
   </si>
 </sst>
 </file>
@@ -1591,13 +1597,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ANZ7"/>
+  <dimension ref="A1:AOA7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:B1048576"/>
+      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,65 +1616,66 @@
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" style="1"/>
-    <col min="9" max="9" width="26.85546875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" style="51" customWidth="1"/>
-    <col min="11" max="11" width="24" style="1" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11" style="56" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="56" customWidth="1"/>
-    <col min="15" max="15" width="23.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="1" customWidth="1"/>
-    <col min="17" max="24" width="26.85546875" style="1" customWidth="1"/>
-    <col min="25" max="25" width="23" style="1"/>
-    <col min="26" max="26" width="23" style="56"/>
-    <col min="27" max="27" width="10.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="19" style="56" customWidth="1"/>
-    <col min="29" max="29" width="19.140625" style="56" customWidth="1"/>
-    <col min="30" max="30" width="10.42578125" style="1" customWidth="1"/>
-    <col min="31" max="31" width="11.42578125" style="56" customWidth="1"/>
-    <col min="32" max="32" width="10.42578125" style="1" customWidth="1"/>
-    <col min="33" max="34" width="9.140625" style="1"/>
-    <col min="35" max="35" width="15.28515625" style="1" customWidth="1"/>
-    <col min="36" max="36" width="22.7109375" style="1"/>
-    <col min="37" max="37" width="13" style="1" customWidth="1"/>
-    <col min="38" max="38" width="15.42578125" style="1" customWidth="1"/>
-    <col min="39" max="39" width="22.7109375" style="1"/>
-    <col min="40" max="40" width="9.140625" style="1"/>
-    <col min="41" max="41" width="15.140625" style="1" customWidth="1"/>
-    <col min="42" max="42" width="20.140625" style="1" customWidth="1"/>
-    <col min="43" max="43" width="12.85546875" style="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" style="1"/>
-    <col min="45" max="45" width="11.42578125" style="1" customWidth="1"/>
-    <col min="46" max="47" width="9.140625" style="1"/>
-    <col min="48" max="48" width="22.7109375" style="1"/>
-    <col min="49" max="52" width="9.140625" style="1"/>
-    <col min="53" max="53" width="11.5703125" style="1" customWidth="1"/>
-    <col min="54" max="54" width="12.28515625" style="1" customWidth="1"/>
-    <col min="55" max="57" width="13.5703125" style="1" customWidth="1"/>
-    <col min="58" max="59" width="10.85546875" style="1" customWidth="1"/>
-    <col min="60" max="60" width="15.42578125" style="1" customWidth="1"/>
-    <col min="61" max="61" width="9.28515625" style="1"/>
-    <col min="62" max="62" width="17" style="1" customWidth="1"/>
-    <col min="63" max="63" width="12.28515625" style="1" customWidth="1"/>
-    <col min="64" max="64" width="11.7109375" style="1" customWidth="1"/>
-    <col min="65" max="65" width="16" style="1" customWidth="1"/>
-    <col min="66" max="66" width="9.140625" style="1"/>
-    <col min="67" max="67" width="12" customWidth="1"/>
-    <col min="68" max="72" width="11.85546875" style="1" customWidth="1"/>
-    <col min="73" max="73" width="14.85546875" style="1" customWidth="1"/>
-    <col min="74" max="74" width="12.28515625" style="1" customWidth="1"/>
-    <col min="75" max="76" width="9.140625" style="1"/>
-    <col min="77" max="77" width="18.42578125" style="1" customWidth="1"/>
-    <col min="78" max="78" width="10.140625" style="1" customWidth="1"/>
-    <col min="79" max="1066" width="9.28515625" style="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="51" customWidth="1"/>
+    <col min="12" max="12" width="24" style="1" customWidth="1"/>
+    <col min="13" max="13" width="26.85546875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="11" style="56" customWidth="1"/>
+    <col min="15" max="15" width="10.5703125" style="56" customWidth="1"/>
+    <col min="16" max="16" width="23.85546875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="1" customWidth="1"/>
+    <col min="18" max="25" width="26.85546875" style="1" customWidth="1"/>
+    <col min="26" max="26" width="23" style="1"/>
+    <col min="27" max="27" width="23" style="56"/>
+    <col min="28" max="28" width="10.42578125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="19" style="56" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" style="56" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" style="1" customWidth="1"/>
+    <col min="32" max="32" width="11.42578125" style="56" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" style="1" customWidth="1"/>
+    <col min="34" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="15.28515625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="22.7109375" style="1"/>
+    <col min="38" max="38" width="13" style="1" customWidth="1"/>
+    <col min="39" max="39" width="15.42578125" style="1" customWidth="1"/>
+    <col min="40" max="40" width="22.7109375" style="1"/>
+    <col min="41" max="41" width="9.140625" style="1"/>
+    <col min="42" max="42" width="15.140625" style="1" customWidth="1"/>
+    <col min="43" max="43" width="20.140625" style="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="1" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="1"/>
+    <col min="46" max="46" width="11.42578125" style="1" customWidth="1"/>
+    <col min="47" max="48" width="9.140625" style="1"/>
+    <col min="49" max="49" width="22.7109375" style="1"/>
+    <col min="50" max="53" width="9.140625" style="1"/>
+    <col min="54" max="54" width="11.5703125" style="1" customWidth="1"/>
+    <col min="55" max="55" width="12.28515625" style="1" customWidth="1"/>
+    <col min="56" max="58" width="13.5703125" style="1" customWidth="1"/>
+    <col min="59" max="60" width="10.85546875" style="1" customWidth="1"/>
+    <col min="61" max="61" width="15.42578125" style="1" customWidth="1"/>
+    <col min="62" max="62" width="9.28515625" style="1"/>
+    <col min="63" max="63" width="17" style="1" customWidth="1"/>
+    <col min="64" max="64" width="12.28515625" style="1" customWidth="1"/>
+    <col min="65" max="65" width="11.7109375" style="1" customWidth="1"/>
+    <col min="66" max="66" width="16" style="1" customWidth="1"/>
+    <col min="67" max="67" width="9.140625" style="1"/>
+    <col min="68" max="68" width="12" customWidth="1"/>
+    <col min="69" max="73" width="11.85546875" style="1" customWidth="1"/>
+    <col min="74" max="74" width="14.85546875" style="1" customWidth="1"/>
+    <col min="75" max="75" width="12.28515625" style="1" customWidth="1"/>
+    <col min="76" max="77" width="9.140625" style="1"/>
+    <col min="78" max="78" width="18.42578125" style="1" customWidth="1"/>
+    <col min="79" max="79" width="10.140625" style="1" customWidth="1"/>
+    <col min="80" max="1067" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="2" spans="1:78" s="1" customFormat="1" ht="51.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:79" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>0</v>
       </c>
@@ -1696,22 +1703,22 @@
       <c r="I2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J2" s="48" t="s">
+      <c r="J2" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="48" t="s">
         <v>104</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="M2" s="61" t="s">
+      <c r="L2" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="21" t="s">
         <v>101</v>
       </c>
       <c r="N2" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="21" t="s">
+      <c r="O2" s="61" t="s">
         <v>101</v>
       </c>
       <c r="P2" s="21" t="s">
@@ -1720,8 +1727,8 @@
       <c r="Q2" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>87</v>
+      <c r="R2" s="21" t="s">
+        <v>101</v>
       </c>
       <c r="S2" s="12" t="s">
         <v>87</v>
@@ -1738,44 +1745,44 @@
       <c r="W2" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="X2" s="23" t="s">
-        <v>33</v>
+      <c r="X2" s="12" t="s">
+        <v>87</v>
       </c>
       <c r="Y2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="57" t="s">
+      <c r="Z2" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="57" t="s">
+      <c r="AB2" s="24" t="s">
         <v>33</v>
       </c>
       <c r="AC2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AD2" s="24" t="s">
+      <c r="AD2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="AE2" s="57" t="s">
+      <c r="AE2" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="25" t="s">
-        <v>44</v>
+      <c r="AF2" s="57" t="s">
+        <v>33</v>
       </c>
       <c r="AG2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AH2" s="26" t="s">
+      <c r="AH2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="AI2" s="54" t="s">
+      <c r="AI2" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="AJ2" s="54" t="s">
         <v>91</v>
-      </c>
-      <c r="AJ2" s="22" t="s">
-        <v>1</v>
       </c>
       <c r="AK2" s="22" t="s">
         <v>1</v>
@@ -1826,7 +1833,7 @@
         <v>1</v>
       </c>
       <c r="BA2" s="22" t="s">
-        <v>133</v>
+        <v>1</v>
       </c>
       <c r="BB2" s="22" t="s">
         <v>133</v>
@@ -1849,8 +1856,8 @@
       <c r="BH2" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="BI2" s="32" t="s">
-        <v>69</v>
+      <c r="BI2" s="22" t="s">
+        <v>133</v>
       </c>
       <c r="BJ2" s="32" t="s">
         <v>69</v>
@@ -1861,10 +1868,10 @@
       <c r="BL2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BM2" s="31" t="s">
+      <c r="BM2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BN2" s="32" t="s">
+      <c r="BN2" s="31" t="s">
         <v>69</v>
       </c>
       <c r="BO2" s="32" t="s">
@@ -1885,10 +1892,10 @@
       <c r="BT2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BU2" s="33" t="s">
+      <c r="BU2" s="32" t="s">
         <v>69</v>
       </c>
-      <c r="BV2" s="32" t="s">
+      <c r="BV2" s="33" t="s">
         <v>69</v>
       </c>
       <c r="BW2" s="32" t="s">
@@ -1903,8 +1910,11 @@
       <c r="BZ2" s="32" t="s">
         <v>69</v>
       </c>
+      <c r="CA2" s="32" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="3" spans="1:78" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:79" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
         <v>72</v>
       </c>
@@ -1929,218 +1939,219 @@
       <c r="H3" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="J3" s="49" t="s">
+      <c r="K3" s="49" t="s">
         <v>180</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="L3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M3" s="62" t="s">
+      <c r="N3" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="62" t="s">
+      <c r="O3" s="62" t="s">
         <v>18</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="P3" s="8" t="s">
+      <c r="Q3" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="Q3" s="8" t="s">
+      <c r="R3" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="S3" s="11" t="s">
+      <c r="T3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="T3" s="11" t="s">
+      <c r="U3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="V3" s="10" t="s">
+      <c r="W3" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="W3" s="40" t="s">
+      <c r="X3" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="X3" s="55" t="s">
+      <c r="Y3" s="55" t="s">
         <v>234</v>
       </c>
-      <c r="Y3" s="55" t="s">
+      <c r="Z3" s="55" t="s">
         <v>237</v>
       </c>
-      <c r="Z3" s="60" t="s">
+      <c r="AA3" s="60" t="s">
         <v>99</v>
       </c>
-      <c r="AA3" s="13" t="s">
+      <c r="AB3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AB3" s="58" t="s">
+      <c r="AC3" s="58" t="s">
         <v>89</v>
       </c>
-      <c r="AC3" s="58" t="s">
+      <c r="AD3" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="AD3" s="13" t="s">
+      <c r="AE3" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="AE3" s="58" t="s">
+      <c r="AF3" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="AF3" s="27" t="s">
+      <c r="AG3" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="AG3" s="28" t="s">
+      <c r="AH3" s="28" t="s">
         <v>80</v>
       </c>
-      <c r="AH3" s="27" t="s">
+      <c r="AI3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="AI3" s="30" t="s">
+      <c r="AJ3" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="AJ3" s="30" t="s">
+      <c r="AK3" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="AK3" s="30" t="s">
+      <c r="AL3" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="AL3" s="30" t="s">
+      <c r="AM3" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="AM3" s="30" t="s">
+      <c r="AN3" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="AN3" s="30" t="s">
+      <c r="AO3" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="AO3" s="30" t="s">
+      <c r="AP3" s="30" t="s">
         <v>200</v>
       </c>
-      <c r="AP3" s="30" t="s">
+      <c r="AQ3" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="AQ3" s="30" t="s">
+      <c r="AR3" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="AR3" s="30" t="s">
+      <c r="AS3" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="AS3" s="30" t="s">
+      <c r="AT3" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="AT3" s="30" t="s">
+      <c r="AU3" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="AU3" s="30" t="s">
+      <c r="AV3" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="AV3" s="30" t="s">
+      <c r="AW3" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="AW3" s="30" t="s">
+      <c r="AX3" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="AX3" s="30" t="s">
+      <c r="AY3" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="AY3" s="30" t="s">
+      <c r="AZ3" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="AZ3" s="30" t="s">
+      <c r="BA3" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="BA3" s="30" t="s">
+      <c r="BB3" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="BB3" s="30" t="s">
+      <c r="BC3" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="BC3" s="30" t="s">
+      <c r="BD3" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="BD3" s="30" t="s">
+      <c r="BE3" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="BE3" s="30" t="s">
+      <c r="BF3" s="30" t="s">
         <v>181</v>
       </c>
-      <c r="BF3" s="30" t="s">
+      <c r="BG3" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="BG3" s="30" t="s">
+      <c r="BH3" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="BH3" s="30" t="s">
+      <c r="BI3" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="BI3" s="29" t="s">
+      <c r="BJ3" s="29" t="s">
         <v>152</v>
       </c>
-      <c r="BJ3" s="29" t="s">
+      <c r="BK3" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="BK3" s="29" t="s">
+      <c r="BL3" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="BL3" s="29" t="s">
+      <c r="BM3" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="BM3" s="29" t="s">
+      <c r="BN3" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="BN3" s="29" t="s">
+      <c r="BO3" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="BO3" s="29" t="s">
+      <c r="BP3" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="BP3" s="29" t="s">
+      <c r="BQ3" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="BQ3" s="29" t="s">
+      <c r="BR3" s="29" t="s">
         <v>161</v>
       </c>
-      <c r="BR3" s="29" t="s">
+      <c r="BS3" s="29" t="s">
         <v>162</v>
       </c>
-      <c r="BS3" s="29" t="s">
+      <c r="BT3" s="29" t="s">
         <v>164</v>
       </c>
-      <c r="BT3" s="29" t="s">
+      <c r="BU3" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="BU3" s="29" t="s">
+      <c r="BV3" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="BV3" s="29" t="s">
+      <c r="BW3" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="BW3" s="29" t="s">
+      <c r="BX3" s="29" t="s">
         <v>168</v>
       </c>
-      <c r="BX3" s="29" t="s">
+      <c r="BY3" s="29" t="s">
         <v>170</v>
       </c>
-      <c r="BY3" s="29" t="s">
+      <c r="BZ3" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="BZ3" s="29" t="s">
+      <c r="CA3" s="29" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:78" s="47" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:79" s="47" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="39" t="s">
         <v>5</v>
       </c>
@@ -2166,217 +2177,220 @@
         <v>7</v>
       </c>
       <c r="I4" s="43" t="s">
+        <v>239</v>
+      </c>
+      <c r="J4" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="J4" s="50" t="s">
+      <c r="K4" s="50" t="s">
         <v>144</v>
       </c>
-      <c r="K4" s="43" t="s">
+      <c r="L4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="43" t="s">
+      <c r="M4" s="43" t="s">
         <v>77</v>
       </c>
-      <c r="M4" s="45" t="s">
+      <c r="N4" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="45" t="s">
+      <c r="O4" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="43" t="s">
+      <c r="P4" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="43" t="s">
+      <c r="Q4" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="Q4" s="43" t="s">
+      <c r="R4" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="R4" s="43" t="s">
+      <c r="S4" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="S4" s="43" t="s">
+      <c r="T4" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="T4" s="43" t="s">
+      <c r="U4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="U4" s="43" t="s">
+      <c r="V4" s="43" t="s">
         <v>146</v>
       </c>
-      <c r="V4" s="43" t="s">
+      <c r="W4" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="W4" s="46" t="s">
+      <c r="X4" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="X4" s="43" t="s">
+      <c r="Y4" s="43" t="s">
         <v>235</v>
       </c>
-      <c r="Y4" s="43" t="s">
+      <c r="Z4" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="Z4" s="45" t="s">
+      <c r="AA4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="AA4" s="43" t="s">
+      <c r="AB4" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="AB4" s="45" t="s">
+      <c r="AC4" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="AC4" s="45" t="s">
+      <c r="AD4" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="AD4" s="43" t="s">
+      <c r="AE4" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="AE4" s="45" t="s">
+      <c r="AF4" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="AF4" s="43" t="s">
+      <c r="AG4" s="43" t="s">
         <v>82</v>
       </c>
-      <c r="AG4" s="43" t="s">
+      <c r="AH4" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="AH4" s="43" t="s">
+      <c r="AI4" s="43" t="s">
         <v>46</v>
       </c>
-      <c r="AI4" s="43" t="s">
+      <c r="AJ4" s="43" t="s">
         <v>229</v>
       </c>
-      <c r="AJ4" s="43" t="s">
+      <c r="AK4" s="43" t="s">
         <v>212</v>
       </c>
-      <c r="AK4" s="43" t="s">
+      <c r="AL4" s="43" t="s">
         <v>213</v>
       </c>
-      <c r="AL4" s="43" t="s">
+      <c r="AM4" s="43" t="s">
         <v>214</v>
       </c>
-      <c r="AM4" s="43" t="s">
+      <c r="AN4" s="43" t="s">
         <v>215</v>
       </c>
-      <c r="AN4" s="43" t="s">
+      <c r="AO4" s="43" t="s">
         <v>216</v>
       </c>
-      <c r="AO4" s="43" t="s">
+      <c r="AP4" s="43" t="s">
         <v>217</v>
       </c>
-      <c r="AP4" s="43" t="s">
+      <c r="AQ4" s="43" t="s">
         <v>218</v>
       </c>
-      <c r="AQ4" s="43" t="s">
+      <c r="AR4" s="43" t="s">
         <v>219</v>
       </c>
-      <c r="AR4" s="43" t="s">
+      <c r="AS4" s="43" t="s">
         <v>230</v>
       </c>
-      <c r="AS4" s="43" t="s">
+      <c r="AT4" s="43" t="s">
         <v>231</v>
       </c>
-      <c r="AT4" s="43" t="s">
+      <c r="AU4" s="43" t="s">
         <v>232</v>
       </c>
-      <c r="AU4" s="43" t="s">
+      <c r="AV4" s="43" t="s">
         <v>220</v>
       </c>
-      <c r="AV4" s="43" t="s">
+      <c r="AW4" s="43" t="s">
         <v>221</v>
       </c>
-      <c r="AW4" s="43" t="s">
+      <c r="AX4" s="43" t="s">
         <v>222</v>
       </c>
-      <c r="AX4" s="43" t="s">
+      <c r="AY4" s="43" t="s">
         <v>223</v>
       </c>
-      <c r="AY4" s="43" t="s">
+      <c r="AZ4" s="43" t="s">
         <v>225</v>
       </c>
-      <c r="AZ4" s="43" t="s">
+      <c r="BA4" s="43" t="s">
         <v>224</v>
       </c>
-      <c r="BA4" s="43" t="s">
+      <c r="BB4" s="43" t="s">
         <v>182</v>
       </c>
-      <c r="BB4" s="43" t="s">
+      <c r="BC4" s="43" t="s">
         <v>136</v>
       </c>
-      <c r="BC4" s="43" t="s">
+      <c r="BD4" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="BD4" s="43" t="s">
+      <c r="BE4" s="43" t="s">
         <v>184</v>
       </c>
-      <c r="BE4" s="43" t="s">
+      <c r="BF4" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="BF4" s="43" t="s">
+      <c r="BG4" s="43" t="s">
         <v>138</v>
       </c>
-      <c r="BG4" s="43" t="s">
+      <c r="BH4" s="43" t="s">
         <v>139</v>
       </c>
-      <c r="BH4" s="43" t="s">
+      <c r="BI4" s="43" t="s">
         <v>185</v>
       </c>
-      <c r="BI4" s="43" t="s">
+      <c r="BJ4" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="BJ4" s="43" t="s">
+      <c r="BK4" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="BK4" s="46" t="s">
+      <c r="BL4" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="BL4" s="43" t="s">
+      <c r="BM4" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="BM4" s="43" t="s">
+      <c r="BN4" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="BN4" s="46" t="s">
+      <c r="BO4" s="46" t="s">
         <v>62</v>
       </c>
-      <c r="BO4" s="46" t="s">
+      <c r="BP4" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="BP4" s="46" t="s">
+      <c r="BQ4" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="BQ4" s="46" t="s">
+      <c r="BR4" s="46" t="s">
         <v>64</v>
       </c>
-      <c r="BR4" s="43" t="s">
+      <c r="BS4" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="BS4" s="43" t="s">
+      <c r="BT4" s="43" t="s">
         <v>128</v>
       </c>
-      <c r="BT4" s="43" t="s">
+      <c r="BU4" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="BU4" s="46" t="s">
+      <c r="BV4" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="BV4" s="43" t="s">
+      <c r="BW4" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="BW4" s="46" t="s">
+      <c r="BX4" s="46" t="s">
         <v>68</v>
       </c>
-      <c r="BX4" s="43" t="s">
+      <c r="BY4" s="43" t="s">
         <v>92</v>
       </c>
-      <c r="BY4" s="46" t="s">
+      <c r="BZ4" s="46" t="s">
         <v>67</v>
       </c>
-      <c r="BZ4" s="46" t="s">
+      <c r="CA4" s="46" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:78" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:79" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
         <v>71</v>
       </c>
@@ -2401,237 +2415,240 @@
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="J5" s="52" t="s">
+      <c r="K5" s="52" t="s">
         <v>177</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="M5" s="59" t="s">
+      <c r="N5" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="O5" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="P5" s="4" t="s">
+      <c r="Q5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Q5" s="4" t="s">
+      <c r="R5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="R5" s="4" t="s">
+      <c r="S5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="U5" s="4" t="s">
+      <c r="V5" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="V5" s="4" t="s">
+      <c r="W5" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="W5" s="4" t="s">
+      <c r="X5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="X5" s="4" t="s">
+      <c r="Y5" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="Y5" s="4" t="s">
+      <c r="Z5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Z5" s="59" t="s">
+      <c r="AA5" s="59" t="s">
         <v>100</v>
       </c>
-      <c r="AA5" s="4" t="s">
+      <c r="AB5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AB5" s="59" t="s">
+      <c r="AC5" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="AC5" s="59" t="s">
+      <c r="AD5" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="AD5" s="4" t="s">
+      <c r="AE5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AE5" s="59" t="s">
+      <c r="AF5" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="AF5" s="4" t="s">
+      <c r="AG5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AG5" s="4" t="s">
+      <c r="AH5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AH5" s="4" t="s">
+      <c r="AI5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AI5" s="4" t="s">
+      <c r="AJ5" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="AJ5" s="4" t="s">
+      <c r="AK5" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AM5" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="AN5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AP5" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="AR5" s="4" t="s">
+      <c r="AS5" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="AS5" s="4" t="s">
+      <c r="AT5" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="AT5" s="4" t="s">
+      <c r="AU5" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="AU5" s="4" t="s">
+      <c r="AV5" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="AV5" s="4" t="s">
+      <c r="AW5" s="4" t="s">
         <v>210</v>
       </c>
-      <c r="AW5" s="4" t="s">
+      <c r="AX5" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="AX5" s="4" t="s">
+      <c r="AY5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="AZ5" s="4" t="s">
+      <c r="BA5" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="BA5" s="4" t="s">
+      <c r="BB5" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="BB5" s="4" t="s">
+      <c r="BC5" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="BC5" s="4" t="s">
+      <c r="BD5" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="BD5" s="4" t="s">
+      <c r="BE5" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="BE5" s="4" t="s">
+      <c r="BF5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="BF5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BH5" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="BH5" s="4" t="s">
+      <c r="BI5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="BI5" s="4" t="s">
+      <c r="BJ5" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="BJ5" s="4" t="s">
+      <c r="BK5" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="BK5" s="7" t="s">
+      <c r="BL5" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="BL5" s="4" t="s">
+      <c r="BM5" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="BM5" s="4" t="s">
+      <c r="BN5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="BN5" s="7" t="s">
+      <c r="BO5" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="BO5" s="42" t="s">
+      <c r="BP5" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="BP5" s="7" t="s">
+      <c r="BQ5" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="BQ5" s="7" t="s">
+      <c r="BR5" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="BR5" s="4" t="s">
+      <c r="BS5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="BS5" s="4" t="s">
+      <c r="BT5" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="BT5" s="4" t="s">
+      <c r="BU5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="BU5" s="14" t="s">
+      <c r="BV5" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="BV5" s="4" t="s">
+      <c r="BW5" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="BW5" s="7" t="s">
+      <c r="BX5" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="BX5" s="4" t="s">
+      <c r="BY5" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="BY5" s="7" t="s">
+      <c r="BZ5" s="7" t="s">
         <v>173</v>
       </c>
-      <c r="BZ5" s="7" t="s">
+      <c r="CA5" s="7" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:79" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.25">
       <c r="G7" s="35"/>
     </row>
   </sheetData>
   <dataValidations count="5">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H1048576">
-      <formula1>"Class,Collection,File,Fonds,Item,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
+      <formula1>"Class,Collection,File,Fonds,Item,Other Level,Record Group,Series,Sub-Fonds,Sub-Group,Sub-Series"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K6:K1048576">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O6:O1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P6:P1048576">
       <formula1>"bulk,single,inclusive"</formula1>
     </dataValidation>
     <dataValidation type="whole" showInputMessage="1" showErrorMessage="1" sqref="G6:G1048576">
       <formula1>1</formula1>
       <formula2>20</formula2>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I6:I1048576">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J6:J1048576">
       <formula1>"FALSE,TRUE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
change field name from 'Thumbnail' to 'thumbnail'
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -160,9 +160,6 @@
     <t>digital_object_link</t>
   </si>
   <si>
-    <t>Thumbnail</t>
-  </si>
-  <si>
     <t>URL of Linked-out digital object</t>
   </si>
   <si>
@@ -729,6 +726,9 @@
   </si>
   <si>
     <t>Other Level</t>
+  </si>
+  <si>
+    <t>thumbnail (onLoad, embed)</t>
   </si>
 </sst>
 </file>
@@ -1578,10 +1578,10 @@
   <dimension ref="A1:AOA7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="AI4" sqref="AI4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1650,7 +1650,7 @@
   <sheetData>
     <row r="1" spans="1:79" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:79" s="1" customFormat="1" ht="64.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -1658,73 +1658,73 @@
         <v>0</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C2" s="16" t="s">
-        <v>105</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="K2" s="47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="N2" s="60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O2" s="60" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="W2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="Y2" s="23" t="s">
         <v>33</v>
@@ -1760,7 +1760,7 @@
         <v>44</v>
       </c>
       <c r="AJ2" s="53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="AK2" s="22" t="s">
         <v>1</v>
@@ -1814,115 +1814,115 @@
         <v>1</v>
       </c>
       <c r="BB2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BC2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BD2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BE2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BF2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BG2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BH2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BI2" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="BJ2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BK2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BL2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BM2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BN2" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BO2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BP2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BQ2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BR2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BS2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BT2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BU2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BV2" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BW2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BX2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BY2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="BZ2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="CA2" s="32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:79" ht="217.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="37" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F3" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I3" s="17"/>
       <c r="J3" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K3" s="48" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>2</v>
@@ -1937,16 +1937,16 @@
         <v>18</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>19</v>
       </c>
       <c r="R3" s="8" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="S3" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="T3" s="11" t="s">
         <v>22</v>
@@ -1955,178 +1955,178 @@
         <v>24</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="W3" s="10" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="X3" s="40" t="s">
         <v>39</v>
       </c>
       <c r="Y3" s="54" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Z3" s="54" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AA3" s="59" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AB3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="AC3" s="57" t="s">
+        <v>88</v>
+      </c>
+      <c r="AD3" s="57" t="s">
+        <v>96</v>
+      </c>
+      <c r="AE3" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="AD3" s="57" t="s">
+      <c r="AF3" s="57" t="s">
         <v>97</v>
       </c>
-      <c r="AE3" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AF3" s="57" t="s">
-        <v>98</v>
-      </c>
       <c r="AG3" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AH3" s="28" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AI3" s="27" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AJ3" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="AK3" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL3" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="AM3" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="AN3" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="AO3" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="AP3" s="30" t="s">
+        <v>192</v>
+      </c>
+      <c r="AQ3" s="30" t="s">
+        <v>194</v>
+      </c>
+      <c r="AR3" s="30" t="s">
+        <v>191</v>
+      </c>
+      <c r="AS3" s="30" t="s">
         <v>193</v>
       </c>
-      <c r="AK3" s="30" t="s">
+      <c r="AT3" s="30" t="s">
         <v>195</v>
       </c>
-      <c r="AL3" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="AM3" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="AN3" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="AO3" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="AP3" s="30" t="s">
-        <v>193</v>
-      </c>
-      <c r="AQ3" s="30" t="s">
-        <v>195</v>
-      </c>
-      <c r="AR3" s="30" t="s">
-        <v>192</v>
-      </c>
-      <c r="AS3" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="AT3" s="30" t="s">
+      <c r="AU3" s="30" t="s">
+        <v>197</v>
+      </c>
+      <c r="AV3" s="30" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW3" s="30" t="s">
         <v>196</v>
       </c>
-      <c r="AU3" s="30" t="s">
+      <c r="AX3" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="AY3" s="30" t="s">
         <v>198</v>
       </c>
-      <c r="AV3" s="30" t="s">
+      <c r="AZ3" s="30" t="s">
+        <v>196</v>
+      </c>
+      <c r="BA3" s="30" t="s">
         <v>199</v>
       </c>
-      <c r="AW3" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="AX3" s="30" t="s">
-        <v>200</v>
-      </c>
-      <c r="AY3" s="30" t="s">
-        <v>199</v>
-      </c>
-      <c r="AZ3" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="BA3" s="30" t="s">
-        <v>200</v>
-      </c>
       <c r="BB3" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BC3" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="BD3" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="BD3" s="30" t="s">
-        <v>128</v>
-      </c>
       <c r="BE3" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BF3" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="BG3" s="30" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH3" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="BH3" s="30" t="s">
-        <v>128</v>
-      </c>
       <c r="BI3" s="30" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="BJ3" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="BK3" s="29" t="s">
         <v>145</v>
       </c>
-      <c r="BK3" s="29" t="s">
+      <c r="BL3" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="BL3" s="29" t="s">
+      <c r="BM3" s="29" t="s">
         <v>147</v>
       </c>
-      <c r="BM3" s="29" t="s">
+      <c r="BN3" s="29" t="s">
         <v>148</v>
       </c>
-      <c r="BN3" s="29" t="s">
+      <c r="BO3" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="BO3" s="29" t="s">
+      <c r="BP3" s="29" t="s">
         <v>150</v>
       </c>
-      <c r="BP3" s="29" t="s">
+      <c r="BQ3" s="29" t="s">
         <v>151</v>
       </c>
-      <c r="BQ3" s="29" t="s">
-        <v>152</v>
-      </c>
       <c r="BR3" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="BS3" s="29" t="s">
         <v>154</v>
       </c>
-      <c r="BS3" s="29" t="s">
-        <v>155</v>
-      </c>
       <c r="BT3" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="BU3" s="29" t="s">
         <v>157</v>
       </c>
-      <c r="BU3" s="29" t="s">
+      <c r="BV3" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="BV3" s="29" t="s">
+      <c r="BW3" s="29" t="s">
         <v>159</v>
       </c>
-      <c r="BW3" s="29" t="s">
+      <c r="BX3" s="29" t="s">
         <v>160</v>
       </c>
-      <c r="BX3" s="29" t="s">
-        <v>161</v>
-      </c>
       <c r="BY3" s="29" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="BZ3" s="29" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="CA3" s="29" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:79" s="46" customFormat="1" ht="41.85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2137,16 +2137,16 @@
         <v>6</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D4" s="44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="42" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G4" s="42" t="s">
         <v>43</v>
@@ -2155,19 +2155,19 @@
         <v>7</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K4" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="L4" s="42" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="42" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="N4" s="44" t="s">
         <v>26</v>
@@ -2182,10 +2182,10 @@
         <v>25</v>
       </c>
       <c r="R4" s="42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T4" s="42" t="s">
         <v>23</v>
@@ -2194,7 +2194,7 @@
         <v>14</v>
       </c>
       <c r="V4" s="42" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="W4" s="42" t="s">
         <v>41</v>
@@ -2203,7 +2203,7 @@
         <v>40</v>
       </c>
       <c r="Y4" s="42" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="Z4" s="42" t="s">
         <v>9</v>
@@ -2227,186 +2227,186 @@
         <v>37</v>
       </c>
       <c r="AG4" s="42" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AH4" s="42" t="s">
         <v>45</v>
       </c>
       <c r="AI4" s="42" t="s">
-        <v>46</v>
+        <v>233</v>
       </c>
       <c r="AJ4" s="42" t="s">
+        <v>221</v>
+      </c>
+      <c r="AK4" s="42" t="s">
+        <v>204</v>
+      </c>
+      <c r="AL4" s="42" t="s">
+        <v>205</v>
+      </c>
+      <c r="AM4" s="42" t="s">
+        <v>206</v>
+      </c>
+      <c r="AN4" s="42" t="s">
+        <v>207</v>
+      </c>
+      <c r="AO4" s="42" t="s">
+        <v>208</v>
+      </c>
+      <c r="AP4" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="AQ4" s="42" t="s">
+        <v>210</v>
+      </c>
+      <c r="AR4" s="42" t="s">
+        <v>211</v>
+      </c>
+      <c r="AS4" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="AK4" s="42" t="s">
-        <v>205</v>
-      </c>
-      <c r="AL4" s="42" t="s">
-        <v>206</v>
-      </c>
-      <c r="AM4" s="42" t="s">
-        <v>207</v>
-      </c>
-      <c r="AN4" s="42" t="s">
-        <v>208</v>
-      </c>
-      <c r="AO4" s="42" t="s">
-        <v>209</v>
-      </c>
-      <c r="AP4" s="42" t="s">
-        <v>210</v>
-      </c>
-      <c r="AQ4" s="42" t="s">
-        <v>211</v>
-      </c>
-      <c r="AR4" s="42" t="s">
+      <c r="AT4" s="42" t="s">
+        <v>223</v>
+      </c>
+      <c r="AU4" s="42" t="s">
+        <v>224</v>
+      </c>
+      <c r="AV4" s="42" t="s">
         <v>212</v>
       </c>
-      <c r="AS4" s="42" t="s">
-        <v>223</v>
-      </c>
-      <c r="AT4" s="42" t="s">
-        <v>224</v>
-      </c>
-      <c r="AU4" s="42" t="s">
-        <v>225</v>
-      </c>
-      <c r="AV4" s="42" t="s">
+      <c r="AW4" s="42" t="s">
         <v>213</v>
       </c>
-      <c r="AW4" s="42" t="s">
+      <c r="AX4" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="AX4" s="42" t="s">
+      <c r="AY4" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="AY4" s="42" t="s">
+      <c r="AZ4" s="42" t="s">
+        <v>217</v>
+      </c>
+      <c r="BA4" s="42" t="s">
         <v>216</v>
       </c>
-      <c r="AZ4" s="42" t="s">
-        <v>218</v>
-      </c>
-      <c r="BA4" s="42" t="s">
-        <v>217</v>
-      </c>
       <c r="BB4" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="BC4" s="42" t="s">
+        <v>128</v>
+      </c>
+      <c r="BD4" s="42" t="s">
+        <v>129</v>
+      </c>
+      <c r="BE4" s="42" t="s">
+        <v>176</v>
+      </c>
+      <c r="BF4" s="42" t="s">
         <v>175</v>
       </c>
-      <c r="BC4" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="BD4" s="42" t="s">
+      <c r="BG4" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="BE4" s="42" t="s">
+      <c r="BH4" s="42" t="s">
+        <v>131</v>
+      </c>
+      <c r="BI4" s="42" t="s">
         <v>177</v>
       </c>
-      <c r="BF4" s="42" t="s">
-        <v>176</v>
-      </c>
-      <c r="BG4" s="42" t="s">
-        <v>131</v>
-      </c>
-      <c r="BH4" s="42" t="s">
-        <v>132</v>
-      </c>
-      <c r="BI4" s="42" t="s">
-        <v>178</v>
-      </c>
       <c r="BJ4" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="BK4" s="42" t="s">
+        <v>59</v>
+      </c>
+      <c r="BL4" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="BM4" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="BN4" s="42" t="s">
+        <v>58</v>
+      </c>
+      <c r="BO4" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="BP4" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="BQ4" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="BR4" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="BS4" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="BT4" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="BU4" s="42" t="s">
+        <v>121</v>
+      </c>
+      <c r="BV4" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="BW4" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="BK4" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="BL4" s="45" t="s">
-        <v>63</v>
-      </c>
-      <c r="BM4" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="BN4" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="BO4" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP4" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="BQ4" s="45" t="s">
+      <c r="BX4" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="BY4" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="BZ4" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="BR4" s="45" t="s">
+      <c r="CA4" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="BS4" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="BT4" s="42" t="s">
-        <v>121</v>
-      </c>
-      <c r="BU4" s="42" t="s">
-        <v>122</v>
-      </c>
-      <c r="BV4" s="45" t="s">
-        <v>93</v>
-      </c>
-      <c r="BW4" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="BX4" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="BY4" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="BZ4" s="45" t="s">
-        <v>67</v>
-      </c>
-      <c r="CA4" s="45" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:79" ht="57.4" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="62" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>3</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>15</v>
       </c>
       <c r="I5" s="63" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J5" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="K5" s="51" t="s">
         <v>169</v>
-      </c>
-      <c r="K5" s="51" t="s">
-        <v>170</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>16</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="N5" s="58" t="s">
         <v>28</v>
@@ -2421,10 +2421,10 @@
         <v>19</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T5" s="6" t="s">
         <v>22</v>
@@ -2433,22 +2433,22 @@
         <v>31</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="X5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="Z5" s="4" t="s">
         <v>32</v>
       </c>
       <c r="AA5" s="58" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AB5" s="4" t="s">
         <v>34</v>
@@ -2457,154 +2457,154 @@
         <v>35</v>
       </c>
       <c r="AD5" s="58" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="AE5" s="4" t="s">
         <v>38</v>
       </c>
       <c r="AF5" s="58" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG5" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AH5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AI5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AI5" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="AJ5" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="AK5" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="AK5" s="4" t="s">
+      <c r="AL5" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AL5" s="4" t="s">
+      <c r="AM5" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="AM5" s="4" t="s">
+      <c r="AN5" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="AN5" s="4" t="s">
+      <c r="AO5" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="AO5" s="4" t="s">
+      <c r="AP5" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="AP5" s="4" t="s">
+      <c r="AQ5" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="AQ5" s="4" t="s">
+      <c r="AR5" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="AR5" s="4" t="s">
-        <v>191</v>
-      </c>
       <c r="AS5" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AT5" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="AU5" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="AU5" s="4" t="s">
+      <c r="AV5" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW5" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="AV5" s="4" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW5" s="4" t="s">
-        <v>203</v>
-      </c>
       <c r="AX5" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AY5" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="AY5" s="4" t="s">
+      <c r="AZ5" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="AZ5" s="4" t="s">
-        <v>221</v>
-      </c>
       <c r="BA5" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="BB5" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="BC5" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="BD5" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="BE5" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="BF5" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="BC5" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="BD5" s="4" t="s">
+      <c r="BG5" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="BE5" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="BF5" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="BG5" s="4" t="s">
+      <c r="BH5" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="BH5" s="4" t="s">
-        <v>136</v>
-      </c>
       <c r="BI5" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BJ5" s="4" t="s">
         <v>42</v>
       </c>
       <c r="BK5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="BL5" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="BM5" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="BN5" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="BO5" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="BP5" s="41" t="s">
         <v>4</v>
       </c>
       <c r="BQ5" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="BR5" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="BS5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="BT5" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="BU5" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="BV5" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="BW5" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="BX5" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="BY5" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="BZ5" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="CA5" s="7" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:79" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2651,42 +2651,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="52" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Freeze panels so field name is visible
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -1577,11 +1577,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AOA7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AI4" sqref="AI4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
adjust some column widths
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -1580,24 +1580,24 @@
     <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" style="34" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="34" customWidth="1"/>
     <col min="2" max="2" width="0" style="18" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="17.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" style="1"/>
+    <col min="8" max="8" width="15.42578125" style="1" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="26.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" style="50" customWidth="1"/>
-    <col min="12" max="12" width="24" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="20.42578125" style="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="55" customWidth="1"/>
     <col min="15" max="15" width="10.5703125" style="55" customWidth="1"/>
     <col min="16" max="16" width="23.85546875" style="1" customWidth="1"/>

</xml_diff>

<commit_message>
remove extraneous text from thumbnail column
</commit_message>
<xml_diff>
--- a/templates/aspace_import_excel_template.xlsx
+++ b/templates/aspace_import_excel_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16020" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17610" windowHeight="8955"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -728,7 +728,7 @@
     <t>Other Level</t>
   </si>
   <si>
-    <t>thumbnail (onLoad, embed)</t>
+    <t>thumbnail</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1579,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>